<commit_message>
Adjust hierarchy test config
</commit_message>
<xml_diff>
--- a/dev-page/configs/sparnatural-hierarchy-config.xlsx
+++ b/dev-page/configs/sparnatural-hierarchy-config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="304">
   <si>
     <r>
       <rPr>
@@ -467,6 +467,15 @@
   </si>
   <si>
     <t xml:space="preserve">Juriste investi d'une mission d'autorité publique, qui prépare des contrats sous la forme authentique, pour le compte de ses clients. En tout 1079 notaires ont exercé au sein des quarante études notariales parisiennes dont les archives sont décrites ici.</t>
+  </si>
+  <si>
+    <t>this:NotaireDeParis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notary from parie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notaire de Paris</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;--- Don't touch this cell</t>
@@ -1289,7 +1298,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="68">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1363,20 +1372,19 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="15" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1407,10 +1415,6 @@
     </xf>
     <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3377,7 +3381,7 @@
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
     </row>
-    <row r="11" ht="51">
+    <row r="11" ht="25.5">
       <c r="A11" s="29" t="s">
         <v>69</v>
       </c>
@@ -3410,11 +3414,11 @@
       </c>
       <c r="K11" s="34"/>
       <c r="N11" s="33"/>
-      <c r="O11" s="35" t="s">
+      <c r="O11" s="33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" ht="89.25">
+    <row r="12" ht="25.5">
       <c r="A12" s="29" t="s">
         <v>76</v>
       </c>
@@ -3447,11 +3451,11 @@
       </c>
       <c r="K12" s="34"/>
       <c r="N12" s="33"/>
-      <c r="O12" s="36" t="s">
+      <c r="O12" s="35" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" ht="51">
+    <row r="13" ht="25.5">
       <c r="A13" s="29" t="s">
         <v>83</v>
       </c>
@@ -3467,7 +3471,7 @@
       <c r="E13" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>66</v>
       </c>
       <c r="G13" s="31" t="s">
@@ -3486,25 +3490,25 @@
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
       <c r="N13" s="33"/>
-      <c r="O13" s="36" t="s">
+      <c r="O13" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="37"/>
-      <c r="T13" s="37"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-      <c r="X13" s="37"/>
-      <c r="Y13" s="37"/>
-      <c r="Z13" s="37"/>
-      <c r="AA13" s="37"/>
-      <c r="AB13" s="37"/>
-      <c r="AC13" s="37"/>
-      <c r="AD13" s="37"/>
-      <c r="AE13" s="37"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="36"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="36"/>
+      <c r="W13" s="36"/>
+      <c r="X13" s="36"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="36"/>
+      <c r="AA13" s="36"/>
+      <c r="AB13" s="36"/>
+      <c r="AC13" s="36"/>
+      <c r="AD13" s="36"/>
+      <c r="AE13" s="36"/>
     </row>
     <row r="14" ht="51">
       <c r="A14" s="29" t="s">
@@ -3522,7 +3526,7 @@
       <c r="E14" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="35" t="s">
         <v>66</v>
       </c>
       <c r="G14" s="31" t="s">
@@ -3541,23 +3545,23 @@
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
       <c r="N14" s="33"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="37"/>
-      <c r="AB14" s="37"/>
-      <c r="AC14" s="37"/>
-      <c r="AD14" s="37"/>
-      <c r="AE14" s="37"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="36"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
+      <c r="AA14" s="36"/>
+      <c r="AB14" s="36"/>
+      <c r="AC14" s="36"/>
+      <c r="AD14" s="36"/>
+      <c r="AE14" s="36"/>
     </row>
     <row r="15" ht="51">
       <c r="A15" s="29" t="s">
@@ -3575,7 +3579,7 @@
       <c r="E15" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="35" t="s">
         <v>66</v>
       </c>
       <c r="G15" s="31" t="s">
@@ -3625,7 +3629,7 @@
       <c r="D16" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="38" t="s">
+      <c r="E16" s="29" t="s">
         <v>105</v>
       </c>
       <c r="F16" s="29" t="s">
@@ -3643,7 +3647,6 @@
       <c r="J16" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="K16"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
       <c r="N16" s="33"/>
@@ -3662,10 +3665,10 @@
       <c r="D17" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="29" t="s">
         <v>66</v>
       </c>
       <c r="G17" s="31" t="s">
@@ -3674,7 +3677,7 @@
       <c r="H17" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="37" t="s">
         <v>115</v>
       </c>
       <c r="J17" s="31" t="s">
@@ -3684,7 +3687,7 @@
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="N17" s="33"/>
-      <c r="O17" s="36" t="s">
+      <c r="O17" s="35" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3701,10 +3704,10 @@
       <c r="D18" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="38" t="s">
+      <c r="E18" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="38" t="s">
+      <c r="F18" s="29" t="s">
         <v>66</v>
       </c>
       <c r="G18" s="31" t="s">
@@ -3713,7 +3716,7 @@
       <c r="H18" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="I18" s="39" t="s">
+      <c r="I18" s="37" t="s">
         <v>122</v>
       </c>
       <c r="J18" s="31" t="s">
@@ -3725,7 +3728,7 @@
       <c r="N18" s="33"/>
       <c r="O18" s="33"/>
     </row>
-    <row r="19" ht="89.25">
+    <row r="19" ht="76.5">
       <c r="A19" s="29" t="s">
         <v>124</v>
       </c>
@@ -3738,7 +3741,7 @@
       <c r="D19" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="38" t="s">
+      <c r="E19" s="29" t="s">
         <v>126</v>
       </c>
       <c r="F19" s="29" t="s">
@@ -3750,7 +3753,7 @@
       <c r="H19" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="37" t="s">
         <v>129</v>
       </c>
       <c r="J19" s="31" t="s">
@@ -3758,23 +3761,46 @@
       </c>
       <c r="K19" s="34"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="40"/>
+      <c r="M19" s="38"/>
       <c r="N19" s="33"/>
-      <c r="O19" s="35" t="s">
+      <c r="O19" s="33" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="20" ht="15">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
+      <c r="A20" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="29">
+        <v>7</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>125</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" s="37"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="39" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="21" ht="15"/>
     <row r="22" ht="15">
@@ -6386,21 +6412,21 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="42" t="str">
+      <c r="B1" s="41" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45"/>
+      <c r="C1" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="44"/>
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
@@ -6412,11 +6438,11 @@
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -6428,11 +6454,11 @@
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
@@ -6444,11 +6470,11 @@
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="17"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23"/>
@@ -6461,7 +6487,7 @@
       <c r="B5" s="23"/>
       <c r="C5" s="17"/>
       <c r="G5" s="23"/>
-      <c r="H5" s="39"/>
+      <c r="H5" s="37"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
@@ -6471,74 +6497,74 @@
     </row>
     <row r="6" ht="191.25" hidden="1">
       <c r="A6" s="24" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="M6" s="24" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="N6" s="24"/>
       <c r="O6" s="24" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="P6" s="24" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="R6" s="24" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="S6" s="24" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="T6" s="24" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="U6" s="24" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="V6" s="24" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="W6" s="24" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="X6" s="24" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="Y6" s="24"/>
       <c r="Z6" s="24"/>
@@ -6550,19 +6576,19 @@
         <v>47</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="G7" s="26" t="s">
         <v>55</v>
@@ -6571,131 +6597,131 @@
         <v>56</v>
       </c>
       <c r="I7" s="26" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="J7" s="26" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="K7" s="26" t="s">
         <v>52</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>61</v>
       </c>
       <c r="N7" s="26" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="O7" s="26" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="P7" s="26" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="Q7" s="26" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="R7" s="26" t="s">
         <v>57</v>
       </c>
       <c r="S7" s="26" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="T7" s="26" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="U7" s="26" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="V7" s="26" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="W7" s="26" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="X7" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="Y7" s="47"/>
-      <c r="Z7" s="47"/>
-      <c r="AA7" s="47"/>
-      <c r="AB7" s="47"/>
+        <v>175</v>
+      </c>
+      <c r="Y7" s="46"/>
+      <c r="Z7" s="46"/>
+      <c r="AA7" s="46"/>
+      <c r="AB7" s="46"/>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="50"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="M8" s="49"/>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="49"/>
-      <c r="Y8" s="49"/>
-      <c r="Z8" s="49"/>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="49"/>
-      <c r="AC8" s="49"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
+      <c r="AB8" s="48"/>
+      <c r="AC8" s="48"/>
     </row>
     <row r="9" ht="25.5">
-      <c r="A9" s="51" t="str">
+      <c r="A9" s="50" t="str">
         <f>CONCATENATE("this:",RIGHT(C9,LEN(C9)-SEARCH(":",C9)),"_",RIGHT(B9,LEN(B9)-SEARCH(":",B9)))</f>
         <v>this:Place_hasOrHadPlaceType</v>
       </c>
-      <c r="B9" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>174</v>
+      <c r="B9" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>177</v>
       </c>
       <c r="D9" s="7">
         <f>D8+1</f>
         <v>1</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>176</v>
-      </c>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51">
+        <v>179</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50">
         <v>1</v>
       </c>
-      <c r="K9" s="51" t="s">
+      <c r="K9" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="51"/>
-      <c r="M9" s="51" t="s">
+      <c r="L9" s="50"/>
+      <c r="M9" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="51"/>
+      <c r="N9" s="50"/>
       <c r="O9" s="30" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P9" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
@@ -6712,17 +6738,17 @@
       <c r="AC9" s="34"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="31"/>
-      <c r="C10" s="53"/>
+      <c r="C10" s="52"/>
       <c r="D10" s="34"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
       <c r="L10" s="34"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -6743,17 +6769,17 @@
       <c r="AC10" s="34"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="33"/>
-      <c r="C11" s="53"/>
+      <c r="C11" s="52"/>
       <c r="D11" s="34"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="31"/>
-      <c r="H11" s="54"/>
+      <c r="H11" s="53"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
-      <c r="K11" s="51"/>
+      <c r="K11" s="50"/>
       <c r="L11" s="34"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -6774,17 +6800,17 @@
       <c r="AC11" s="34"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="51"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="31"/>
-      <c r="C12" s="53"/>
+      <c r="C12" s="52"/>
       <c r="D12" s="34"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
-      <c r="H12" s="54"/>
+      <c r="H12" s="53"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="51"/>
+      <c r="K12" s="50"/>
       <c r="L12" s="34"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -6805,51 +6831,51 @@
       <c r="AC12" s="34"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="48" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="50"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
-      <c r="M13" s="49"/>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-      <c r="P13" s="49"/>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="49"/>
-      <c r="U13" s="49"/>
-      <c r="V13" s="49"/>
-      <c r="W13" s="49"/>
-      <c r="X13" s="49"/>
-      <c r="Y13" s="49"/>
-      <c r="Z13" s="49"/>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="49"/>
-      <c r="AC13" s="49"/>
+      <c r="A13" s="47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="48"/>
+      <c r="AC13" s="48"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="54"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="34"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
-      <c r="L14" s="51"/>
+      <c r="L14" s="50"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="30"/>
@@ -6869,47 +6895,47 @@
       <c r="AC14" s="34"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
-      <c r="X15" s="49"/>
-      <c r="Y15" s="49"/>
-      <c r="Z15" s="49"/>
-      <c r="AA15" s="49"/>
-      <c r="AB15" s="49"/>
-      <c r="AC15" s="49"/>
+      <c r="A15" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+      <c r="W15" s="48"/>
+      <c r="X15" s="48"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="48"/>
+      <c r="AB15" s="48"/>
+      <c r="AC15" s="48"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="54"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="34"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -6933,19 +6959,19 @@
       <c r="AC16" s="34"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="54"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="34"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="54"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="34"/>
-      <c r="N17" s="55"/>
+      <c r="N17" s="32"/>
       <c r="O17" s="30"/>
       <c r="P17" s="34"/>
       <c r="Q17" s="30"/>
@@ -6963,19 +6989,19 @@
       <c r="AC17" s="34"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="54"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="34"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="34"/>
-      <c r="N18" s="55"/>
+      <c r="N18" s="32"/>
       <c r="O18" s="30"/>
       <c r="P18" s="34"/>
       <c r="Q18" s="34"/>
@@ -6993,14 +7019,14 @@
       <c r="AC18" s="34"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="31"/>
-      <c r="C19" s="54"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="34"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
-      <c r="H19" s="54"/>
+      <c r="H19" s="53"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -7022,14 +7048,14 @@
       <c r="AC19" s="34"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="31"/>
-      <c r="C20" s="54"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="34"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="54"/>
+      <c r="H20" s="53"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -7053,40 +7079,40 @@
       <c r="AC20" s="34"/>
     </row>
     <row r="21" ht="15.75">
-      <c r="A21" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="49"/>
-      <c r="Z21" s="49"/>
-      <c r="AA21" s="49"/>
-      <c r="AB21" s="49"/>
-      <c r="AC21" s="49"/>
+      <c r="A21" s="47" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" s="49"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="48"/>
+      <c r="AB21" s="48"/>
+      <c r="AC21" s="48"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="34"/>
@@ -7098,8 +7124,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
       <c r="Q22" s="34"/>
@@ -7117,7 +7143,7 @@
       <c r="AC22" s="34"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="34"/>
@@ -7147,79 +7173,79 @@
       <c r="AC23" s="34"/>
     </row>
     <row r="24" ht="15.75">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="47" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="49"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-      <c r="P24" s="49"/>
-      <c r="Q24" s="49"/>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
-      <c r="U24" s="49"/>
-      <c r="V24" s="49"/>
-      <c r="W24" s="49"/>
-      <c r="X24" s="49"/>
-      <c r="Y24" s="49"/>
-      <c r="Z24" s="49"/>
-      <c r="AA24" s="49"/>
-      <c r="AB24" s="49"/>
-      <c r="AC24" s="49"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="48"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="48"/>
+      <c r="S24" s="48"/>
+      <c r="T24" s="48"/>
+      <c r="U24" s="48"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="48"/>
+      <c r="Y24" s="48"/>
+      <c r="Z24" s="48"/>
+      <c r="AA24" s="48"/>
+      <c r="AB24" s="48"/>
+      <c r="AC24" s="48"/>
     </row>
     <row r="25" ht="15">
-      <c r="A25" s="51" t="str">
+      <c r="A25" s="50" t="str">
         <f>CONCATENATE("this:",RIGHT(C25,LEN(C25)-SEARCH(":",C25)),"_",RIGHT(B25,LEN(B25)-SEARCH(":",B25)))</f>
         <v>this:Adresse_hasOrHadLocation</v>
       </c>
-      <c r="B25" s="52" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="53" t="s">
+      <c r="B25" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="52" t="s">
         <v>97</v>
       </c>
       <c r="D25" s="7">
-        <f>D24+1</f>
+        <f t="shared" ref="D25:D29" si="0">D24+1</f>
         <v>1</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>184</v>
-      </c>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="G25" s="53"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51" t="s">
-        <v>185</v>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="O25" s="30" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P25" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q25" s="56" t="s">
-        <v>186</v>
+        <v>181</v>
+      </c>
+      <c r="Q25" s="34" t="s">
+        <v>189</v>
       </c>
       <c r="R25" s="34"/>
       <c r="S25" s="34"/>
@@ -7235,45 +7261,45 @@
       <c r="AC25" s="34"/>
     </row>
     <row r="26" ht="28.5">
-      <c r="A26" s="57" t="s">
-        <v>187</v>
-      </c>
-      <c r="B26" s="52" t="s">
-        <v>188</v>
-      </c>
-      <c r="C26" s="53" t="s">
+      <c r="A26" s="54" t="s">
+        <v>190</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" s="52" t="s">
         <v>97</v>
       </c>
       <c r="D26" s="7">
-        <f>D25+1</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E26" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50" t="s">
+        <v>194</v>
+      </c>
+      <c r="O26" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="P26" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q26" s="34" t="s">
         <v>189</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>190</v>
-      </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51" t="s">
-        <v>191</v>
-      </c>
-      <c r="O26" s="30" t="s">
-        <v>177</v>
-      </c>
-      <c r="P26" s="30" t="s">
-        <v>178</v>
-      </c>
-      <c r="Q26" s="56" t="s">
-        <v>186</v>
       </c>
       <c r="R26" s="34"/>
       <c r="S26" s="34"/>
@@ -7295,78 +7321,78 @@
       <c r="O27" s="7"/>
     </row>
     <row r="28" ht="15.75">
-      <c r="A28" s="48" t="s">
-        <v>192</v>
-      </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="49"/>
-      <c r="R28" s="49"/>
-      <c r="S28" s="49"/>
-      <c r="T28" s="49"/>
-      <c r="U28" s="49"/>
-      <c r="V28" s="49"/>
-      <c r="W28" s="49"/>
-      <c r="X28" s="49"/>
-      <c r="Y28" s="49"/>
-      <c r="Z28" s="49"/>
-      <c r="AA28" s="49"/>
-      <c r="AB28" s="49"/>
-      <c r="AC28" s="49"/>
+      <c r="A28" s="47" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="48"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="48"/>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="48"/>
+      <c r="P28" s="48"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="48"/>
+      <c r="S28" s="48"/>
+      <c r="T28" s="48"/>
+      <c r="U28" s="48"/>
+      <c r="V28" s="48"/>
+      <c r="W28" s="48"/>
+      <c r="X28" s="48"/>
+      <c r="Y28" s="48"/>
+      <c r="Z28" s="48"/>
+      <c r="AA28" s="48"/>
+      <c r="AB28" s="48"/>
+      <c r="AC28" s="48"/>
     </row>
     <row r="29" ht="28.5">
-      <c r="A29" s="57" t="s">
-        <v>193</v>
-      </c>
-      <c r="B29" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>195</v>
+      <c r="A29" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" s="51" t="s">
+        <v>197</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>198</v>
       </c>
       <c r="D29" s="7">
-        <f>D28+1</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51" t="s">
+        <v>200</v>
+      </c>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="L29" s="51"/>
-      <c r="M29" s="51"/>
-      <c r="N29" s="51" t="s">
-        <v>185</v>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="O29" s="30" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="P29" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="Q29" s="34" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="R29" s="34"/>
       <c r="S29" s="34"/>
@@ -9002,18 +9028,18 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="59" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="60" t="s">
-        <v>131</v>
+      <c r="C1" s="57" t="s">
+        <v>134</v>
       </c>
       <c r="D1" s="23"/>
-      <c r="E1" s="60"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -9031,66 +9057,66 @@
       <c r="I2" s="23"/>
     </row>
     <row r="3" ht="91.5" customHeight="1">
-      <c r="A3" s="61" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="61" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="61" t="s">
+      <c r="A3" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="B3" s="58" t="s">
         <v>202</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="C3" s="59" t="s">
         <v>203</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>204</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>206</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D4" s="63" t="s">
-        <v>205</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>206</v>
-      </c>
-      <c r="F4" s="63" t="s">
+      <c r="C4" s="60" t="s">
         <v>207</v>
       </c>
-      <c r="G4" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
+      <c r="D4" s="60" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>209</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="56" t="s">
-        <v>186</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>208</v>
+      <c r="A5" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>211</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -9098,9 +9124,9 @@
       <c r="I5" s="23"/>
     </row>
     <row r="6" ht="276" customHeight="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="23"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
@@ -9109,9 +9135,9 @@
       <c r="I6" s="23"/>
     </row>
     <row r="7" ht="315" customHeight="1">
-      <c r="A7" s="68"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="39"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
@@ -9120,9 +9146,9 @@
       <c r="I7" s="23"/>
     </row>
     <row r="8" ht="333.75" customHeight="1">
-      <c r="A8" s="68"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="39"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
@@ -9132,7 +9158,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="60"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -9143,7 +9169,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="60"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -9154,7 +9180,7 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="60"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -9165,7 +9191,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="60"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -9176,7 +9202,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="60"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -9187,7 +9213,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="60"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -9198,7 +9224,7 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="60"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -9209,7 +9235,7 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="60"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -9220,7 +9246,7 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="60"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -9231,7 +9257,7 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="60"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -9242,7 +9268,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="60"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -9253,7 +9279,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="60"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -9264,7 +9290,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="23"/>
-      <c r="B21" s="60"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -9275,7 +9301,7 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="23"/>
-      <c r="B22" s="60"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -9286,7 +9312,7 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="23"/>
-      <c r="B23" s="60"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -9297,7 +9323,7 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="23"/>
-      <c r="B24" s="60"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -10309,1551 +10335,1551 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="59" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="60" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="69"/>
+      <c r="C1" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="66"/>
       <c r="E1" s="23"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
-      <c r="D2" s="39"/>
+      <c r="D2" s="37"/>
       <c r="E2" s="23"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="39"/>
+      <c r="D3" s="37"/>
       <c r="E3" s="23"/>
     </row>
     <row r="4" ht="58.5" customHeight="1">
-      <c r="A4" s="61" t="s">
-        <v>211</v>
-      </c>
-      <c r="B4" s="61" t="s">
-        <v>212</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="61" t="s">
-        <v>213</v>
+      <c r="A4" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>203</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>216</v>
       </c>
       <c r="E4" s="23"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="63" t="s">
-        <v>204</v>
-      </c>
-      <c r="D5" s="63" t="s">
-        <v>214</v>
-      </c>
-      <c r="E5" s="64"/>
+      <c r="C5" s="60" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" ht="160.5" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="D6" s="39"/>
+        <v>212</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="D6" s="37"/>
       <c r="E6" s="23"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="23"/>
-      <c r="B7" s="60"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="23"/>
-      <c r="D7" s="39"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="23"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="60"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="39"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="23"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="60"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="23"/>
-      <c r="D9" s="39"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="23"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="60"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="39"/>
+      <c r="D10" s="37"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="60"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="39"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="60"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="23"/>
-      <c r="D12" s="39"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="23"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="60"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="23"/>
-      <c r="D13" s="39"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="23"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="60"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="23"/>
-      <c r="D14" s="39"/>
+      <c r="D14" s="37"/>
       <c r="E14" s="23"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="60"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="23"/>
-      <c r="D15" s="39"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="23"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="60"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="23"/>
-      <c r="D16" s="39"/>
+      <c r="D16" s="37"/>
       <c r="E16" s="23"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="60"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="23"/>
-      <c r="D17" s="39"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="23"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="60"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="23"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="37"/>
       <c r="E18" s="23"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="60"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="23"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="37"/>
       <c r="E19" s="23"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="60"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="23"/>
-      <c r="D20" s="39"/>
+      <c r="D20" s="37"/>
       <c r="E20" s="23"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
-      <c r="D21" s="39"/>
+      <c r="D21" s="37"/>
       <c r="E21" s="23"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="37"/>
       <c r="E22" s="23"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
-      <c r="D23" s="39"/>
+      <c r="D23" s="37"/>
       <c r="E23" s="23"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
-      <c r="D24" s="39"/>
+      <c r="D24" s="37"/>
       <c r="E24" s="23"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="23"/>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
-      <c r="D25" s="39"/>
+      <c r="D25" s="37"/>
       <c r="E25" s="23"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="23"/>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
-      <c r="D26" s="39"/>
+      <c r="D26" s="37"/>
       <c r="E26" s="23"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="23"/>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
-      <c r="D27" s="39"/>
+      <c r="D27" s="37"/>
       <c r="E27" s="23"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="23"/>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
-      <c r="D28" s="39"/>
+      <c r="D28" s="37"/>
       <c r="E28" s="23"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="23"/>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
-      <c r="D29" s="39"/>
+      <c r="D29" s="37"/>
       <c r="E29" s="23"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
-      <c r="D30" s="39"/>
+      <c r="D30" s="37"/>
       <c r="E30" s="23"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="23"/>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
-      <c r="D31" s="39"/>
+      <c r="D31" s="37"/>
       <c r="E31" s="23"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
-      <c r="D32" s="39"/>
+      <c r="D32" s="37"/>
       <c r="E32" s="23"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="23"/>
       <c r="B33" s="23"/>
       <c r="C33" s="23"/>
-      <c r="D33" s="39"/>
+      <c r="D33" s="37"/>
       <c r="E33" s="23"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="23"/>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
-      <c r="D34" s="39"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="23"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="23"/>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="39"/>
+      <c r="D35" s="37"/>
       <c r="E35" s="23"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="23"/>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
-      <c r="D36" s="39"/>
+      <c r="D36" s="37"/>
       <c r="E36" s="23"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="23"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
-      <c r="D37" s="39"/>
+      <c r="D37" s="37"/>
       <c r="E37" s="23"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="23"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
-      <c r="D38" s="39"/>
+      <c r="D38" s="37"/>
       <c r="E38" s="23"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="23"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
-      <c r="D39" s="39"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="23"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="23"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
-      <c r="D40" s="39"/>
+      <c r="D40" s="37"/>
       <c r="E40" s="23"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="23"/>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
-      <c r="D41" s="39"/>
+      <c r="D41" s="37"/>
       <c r="E41" s="23"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="23"/>
       <c r="B42" s="23"/>
       <c r="C42" s="23"/>
-      <c r="D42" s="39"/>
+      <c r="D42" s="37"/>
       <c r="E42" s="23"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="23"/>
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
-      <c r="D43" s="39"/>
+      <c r="D43" s="37"/>
       <c r="E43" s="23"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="23"/>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
-      <c r="D44" s="39"/>
+      <c r="D44" s="37"/>
       <c r="E44" s="23"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="23"/>
       <c r="B45" s="23"/>
       <c r="C45" s="23"/>
-      <c r="D45" s="39"/>
+      <c r="D45" s="37"/>
       <c r="E45" s="23"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="23"/>
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
-      <c r="D46" s="39"/>
+      <c r="D46" s="37"/>
       <c r="E46" s="23"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="23"/>
       <c r="B47" s="23"/>
       <c r="C47" s="23"/>
-      <c r="D47" s="39"/>
+      <c r="D47" s="37"/>
       <c r="E47" s="23"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="23"/>
       <c r="B48" s="23"/>
       <c r="C48" s="23"/>
-      <c r="D48" s="39"/>
+      <c r="D48" s="37"/>
       <c r="E48" s="23"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="23"/>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
-      <c r="D49" s="39"/>
+      <c r="D49" s="37"/>
       <c r="E49" s="23"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
       <c r="A50" s="23"/>
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
-      <c r="D50" s="39"/>
+      <c r="D50" s="37"/>
       <c r="E50" s="23"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
       <c r="A51" s="23"/>
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
-      <c r="D51" s="39"/>
+      <c r="D51" s="37"/>
       <c r="E51" s="23"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
       <c r="A52" s="23"/>
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
-      <c r="D52" s="39"/>
+      <c r="D52" s="37"/>
       <c r="E52" s="23"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
       <c r="A53" s="23"/>
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
-      <c r="D53" s="39"/>
+      <c r="D53" s="37"/>
       <c r="E53" s="23"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
       <c r="A54" s="23"/>
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
-      <c r="D54" s="39"/>
+      <c r="D54" s="37"/>
       <c r="E54" s="23"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="23"/>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
-      <c r="D55" s="39"/>
+      <c r="D55" s="37"/>
       <c r="E55" s="23"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="23"/>
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="39"/>
+      <c r="D56" s="37"/>
       <c r="E56" s="23"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
       <c r="A57" s="23"/>
       <c r="B57" s="23"/>
       <c r="C57" s="23"/>
-      <c r="D57" s="39"/>
+      <c r="D57" s="37"/>
       <c r="E57" s="23"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
       <c r="A58" s="23"/>
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
-      <c r="D58" s="39"/>
+      <c r="D58" s="37"/>
       <c r="E58" s="23"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
       <c r="A59" s="23"/>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
-      <c r="D59" s="39"/>
+      <c r="D59" s="37"/>
       <c r="E59" s="23"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
       <c r="A60" s="23"/>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
-      <c r="D60" s="39"/>
+      <c r="D60" s="37"/>
       <c r="E60" s="23"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
       <c r="A61" s="23"/>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
-      <c r="D61" s="39"/>
+      <c r="D61" s="37"/>
       <c r="E61" s="23"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
       <c r="A62" s="23"/>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
-      <c r="D62" s="39"/>
+      <c r="D62" s="37"/>
       <c r="E62" s="23"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
       <c r="A63" s="23"/>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
-      <c r="D63" s="39"/>
+      <c r="D63" s="37"/>
       <c r="E63" s="23"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
-      <c r="D64" s="39"/>
+      <c r="D64" s="37"/>
       <c r="E64" s="23"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
       <c r="A65" s="23"/>
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
-      <c r="D65" s="39"/>
+      <c r="D65" s="37"/>
       <c r="E65" s="23"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
       <c r="A66" s="23"/>
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
-      <c r="D66" s="39"/>
+      <c r="D66" s="37"/>
       <c r="E66" s="23"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
       <c r="C67" s="23"/>
-      <c r="D67" s="39"/>
+      <c r="D67" s="37"/>
       <c r="E67" s="23"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
       <c r="A68" s="23"/>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
-      <c r="D68" s="39"/>
+      <c r="D68" s="37"/>
       <c r="E68" s="23"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
       <c r="A69" s="23"/>
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
-      <c r="D69" s="39"/>
+      <c r="D69" s="37"/>
       <c r="E69" s="23"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
       <c r="A70" s="23"/>
       <c r="B70" s="23"/>
       <c r="C70" s="23"/>
-      <c r="D70" s="39"/>
+      <c r="D70" s="37"/>
       <c r="E70" s="23"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
-      <c r="D71" s="39"/>
+      <c r="D71" s="37"/>
       <c r="E71" s="23"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
       <c r="A72" s="23"/>
       <c r="B72" s="23"/>
       <c r="C72" s="23"/>
-      <c r="D72" s="39"/>
+      <c r="D72" s="37"/>
       <c r="E72" s="23"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="23"/>
       <c r="B73" s="23"/>
       <c r="C73" s="23"/>
-      <c r="D73" s="39"/>
+      <c r="D73" s="37"/>
       <c r="E73" s="23"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
       <c r="A74" s="23"/>
       <c r="B74" s="23"/>
       <c r="C74" s="23"/>
-      <c r="D74" s="39"/>
+      <c r="D74" s="37"/>
       <c r="E74" s="23"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
       <c r="A75" s="23"/>
       <c r="B75" s="23"/>
       <c r="C75" s="23"/>
-      <c r="D75" s="39"/>
+      <c r="D75" s="37"/>
       <c r="E75" s="23"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
       <c r="A76" s="23"/>
       <c r="B76" s="23"/>
       <c r="C76" s="23"/>
-      <c r="D76" s="39"/>
+      <c r="D76" s="37"/>
       <c r="E76" s="23"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
       <c r="A77" s="23"/>
       <c r="B77" s="23"/>
       <c r="C77" s="23"/>
-      <c r="D77" s="39"/>
+      <c r="D77" s="37"/>
       <c r="E77" s="23"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
       <c r="A78" s="23"/>
       <c r="B78" s="23"/>
       <c r="C78" s="23"/>
-      <c r="D78" s="39"/>
+      <c r="D78" s="37"/>
       <c r="E78" s="23"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
       <c r="A79" s="23"/>
       <c r="B79" s="23"/>
       <c r="C79" s="23"/>
-      <c r="D79" s="39"/>
+      <c r="D79" s="37"/>
       <c r="E79" s="23"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
       <c r="A80" s="23"/>
       <c r="B80" s="23"/>
       <c r="C80" s="23"/>
-      <c r="D80" s="39"/>
+      <c r="D80" s="37"/>
       <c r="E80" s="23"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
       <c r="A81" s="23"/>
       <c r="B81" s="23"/>
       <c r="C81" s="23"/>
-      <c r="D81" s="39"/>
+      <c r="D81" s="37"/>
       <c r="E81" s="23"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
       <c r="A82" s="23"/>
       <c r="B82" s="23"/>
       <c r="C82" s="23"/>
-      <c r="D82" s="39"/>
+      <c r="D82" s="37"/>
       <c r="E82" s="23"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
       <c r="A83" s="23"/>
       <c r="B83" s="23"/>
       <c r="C83" s="23"/>
-      <c r="D83" s="39"/>
+      <c r="D83" s="37"/>
       <c r="E83" s="23"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
       <c r="A84" s="23"/>
       <c r="B84" s="23"/>
       <c r="C84" s="23"/>
-      <c r="D84" s="39"/>
+      <c r="D84" s="37"/>
       <c r="E84" s="23"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
       <c r="A85" s="23"/>
       <c r="B85" s="23"/>
       <c r="C85" s="23"/>
-      <c r="D85" s="39"/>
+      <c r="D85" s="37"/>
       <c r="E85" s="23"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
       <c r="A86" s="23"/>
       <c r="B86" s="23"/>
       <c r="C86" s="23"/>
-      <c r="D86" s="39"/>
+      <c r="D86" s="37"/>
       <c r="E86" s="23"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
       <c r="A87" s="23"/>
       <c r="B87" s="23"/>
       <c r="C87" s="23"/>
-      <c r="D87" s="39"/>
+      <c r="D87" s="37"/>
       <c r="E87" s="23"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
       <c r="A88" s="23"/>
       <c r="B88" s="23"/>
       <c r="C88" s="23"/>
-      <c r="D88" s="39"/>
+      <c r="D88" s="37"/>
       <c r="E88" s="23"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
       <c r="A89" s="23"/>
       <c r="B89" s="23"/>
       <c r="C89" s="23"/>
-      <c r="D89" s="39"/>
+      <c r="D89" s="37"/>
       <c r="E89" s="23"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
       <c r="A90" s="23"/>
       <c r="B90" s="23"/>
       <c r="C90" s="23"/>
-      <c r="D90" s="39"/>
+      <c r="D90" s="37"/>
       <c r="E90" s="23"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
       <c r="A91" s="23"/>
       <c r="B91" s="23"/>
       <c r="C91" s="23"/>
-      <c r="D91" s="39"/>
+      <c r="D91" s="37"/>
       <c r="E91" s="23"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
       <c r="A92" s="23"/>
       <c r="B92" s="23"/>
       <c r="C92" s="23"/>
-      <c r="D92" s="39"/>
+      <c r="D92" s="37"/>
       <c r="E92" s="23"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
       <c r="A93" s="23"/>
       <c r="B93" s="23"/>
       <c r="C93" s="23"/>
-      <c r="D93" s="39"/>
+      <c r="D93" s="37"/>
       <c r="E93" s="23"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
       <c r="A94" s="23"/>
       <c r="B94" s="23"/>
       <c r="C94" s="23"/>
-      <c r="D94" s="39"/>
+      <c r="D94" s="37"/>
       <c r="E94" s="23"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
       <c r="A95" s="23"/>
       <c r="B95" s="23"/>
       <c r="C95" s="23"/>
-      <c r="D95" s="39"/>
+      <c r="D95" s="37"/>
       <c r="E95" s="23"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
       <c r="A96" s="23"/>
       <c r="B96" s="23"/>
       <c r="C96" s="23"/>
-      <c r="D96" s="39"/>
+      <c r="D96" s="37"/>
       <c r="E96" s="23"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
       <c r="A97" s="23"/>
       <c r="B97" s="23"/>
       <c r="C97" s="23"/>
-      <c r="D97" s="39"/>
+      <c r="D97" s="37"/>
       <c r="E97" s="23"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
       <c r="A98" s="23"/>
       <c r="B98" s="23"/>
       <c r="C98" s="23"/>
-      <c r="D98" s="39"/>
+      <c r="D98" s="37"/>
       <c r="E98" s="23"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
       <c r="A99" s="23"/>
       <c r="B99" s="23"/>
       <c r="C99" s="23"/>
-      <c r="D99" s="39"/>
+      <c r="D99" s="37"/>
       <c r="E99" s="23"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
       <c r="A100" s="23"/>
       <c r="B100" s="23"/>
       <c r="C100" s="23"/>
-      <c r="D100" s="39"/>
+      <c r="D100" s="37"/>
       <c r="E100" s="23"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
       <c r="A101" s="23"/>
       <c r="B101" s="23"/>
       <c r="C101" s="23"/>
-      <c r="D101" s="39"/>
+      <c r="D101" s="37"/>
       <c r="E101" s="23"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
       <c r="A102" s="23"/>
       <c r="B102" s="23"/>
       <c r="C102" s="23"/>
-      <c r="D102" s="39"/>
+      <c r="D102" s="37"/>
       <c r="E102" s="23"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
       <c r="A103" s="23"/>
       <c r="B103" s="23"/>
       <c r="C103" s="23"/>
-      <c r="D103" s="39"/>
+      <c r="D103" s="37"/>
       <c r="E103" s="23"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
       <c r="A104" s="23"/>
       <c r="B104" s="23"/>
       <c r="C104" s="23"/>
-      <c r="D104" s="39"/>
+      <c r="D104" s="37"/>
       <c r="E104" s="23"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
       <c r="A105" s="23"/>
       <c r="B105" s="23"/>
       <c r="C105" s="23"/>
-      <c r="D105" s="39"/>
+      <c r="D105" s="37"/>
       <c r="E105" s="23"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
       <c r="A106" s="23"/>
       <c r="B106" s="23"/>
       <c r="C106" s="23"/>
-      <c r="D106" s="39"/>
+      <c r="D106" s="37"/>
       <c r="E106" s="23"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
       <c r="A107" s="23"/>
       <c r="B107" s="23"/>
       <c r="C107" s="23"/>
-      <c r="D107" s="39"/>
+      <c r="D107" s="37"/>
       <c r="E107" s="23"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
       <c r="A108" s="23"/>
       <c r="B108" s="23"/>
       <c r="C108" s="23"/>
-      <c r="D108" s="39"/>
+      <c r="D108" s="37"/>
       <c r="E108" s="23"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
       <c r="A109" s="23"/>
       <c r="B109" s="23"/>
       <c r="C109" s="23"/>
-      <c r="D109" s="39"/>
+      <c r="D109" s="37"/>
       <c r="E109" s="23"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
       <c r="A110" s="23"/>
       <c r="B110" s="23"/>
       <c r="C110" s="23"/>
-      <c r="D110" s="39"/>
+      <c r="D110" s="37"/>
       <c r="E110" s="23"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
       <c r="A111" s="23"/>
       <c r="B111" s="23"/>
       <c r="C111" s="23"/>
-      <c r="D111" s="39"/>
+      <c r="D111" s="37"/>
       <c r="E111" s="23"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
       <c r="A112" s="23"/>
       <c r="B112" s="23"/>
       <c r="C112" s="23"/>
-      <c r="D112" s="39"/>
+      <c r="D112" s="37"/>
       <c r="E112" s="23"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
       <c r="A113" s="23"/>
       <c r="B113" s="23"/>
       <c r="C113" s="23"/>
-      <c r="D113" s="39"/>
+      <c r="D113" s="37"/>
       <c r="E113" s="23"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
       <c r="A114" s="23"/>
       <c r="B114" s="23"/>
       <c r="C114" s="23"/>
-      <c r="D114" s="39"/>
+      <c r="D114" s="37"/>
       <c r="E114" s="23"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
       <c r="A115" s="23"/>
       <c r="B115" s="23"/>
       <c r="C115" s="23"/>
-      <c r="D115" s="39"/>
+      <c r="D115" s="37"/>
       <c r="E115" s="23"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
       <c r="A116" s="23"/>
       <c r="B116" s="23"/>
       <c r="C116" s="23"/>
-      <c r="D116" s="39"/>
+      <c r="D116" s="37"/>
       <c r="E116" s="23"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
       <c r="A117" s="23"/>
       <c r="B117" s="23"/>
       <c r="C117" s="23"/>
-      <c r="D117" s="39"/>
+      <c r="D117" s="37"/>
       <c r="E117" s="23"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
       <c r="A118" s="23"/>
       <c r="B118" s="23"/>
       <c r="C118" s="23"/>
-      <c r="D118" s="39"/>
+      <c r="D118" s="37"/>
       <c r="E118" s="23"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
       <c r="A119" s="23"/>
       <c r="B119" s="23"/>
       <c r="C119" s="23"/>
-      <c r="D119" s="39"/>
+      <c r="D119" s="37"/>
       <c r="E119" s="23"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
       <c r="A120" s="23"/>
       <c r="B120" s="23"/>
       <c r="C120" s="23"/>
-      <c r="D120" s="39"/>
+      <c r="D120" s="37"/>
       <c r="E120" s="23"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
       <c r="A121" s="23"/>
       <c r="B121" s="23"/>
       <c r="C121" s="23"/>
-      <c r="D121" s="39"/>
+      <c r="D121" s="37"/>
       <c r="E121" s="23"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
       <c r="A122" s="23"/>
       <c r="B122" s="23"/>
       <c r="C122" s="23"/>
-      <c r="D122" s="39"/>
+      <c r="D122" s="37"/>
       <c r="E122" s="23"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
       <c r="A123" s="23"/>
       <c r="B123" s="23"/>
       <c r="C123" s="23"/>
-      <c r="D123" s="39"/>
+      <c r="D123" s="37"/>
       <c r="E123" s="23"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
       <c r="A124" s="23"/>
       <c r="B124" s="23"/>
       <c r="C124" s="23"/>
-      <c r="D124" s="39"/>
+      <c r="D124" s="37"/>
       <c r="E124" s="23"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
       <c r="A125" s="23"/>
       <c r="B125" s="23"/>
       <c r="C125" s="23"/>
-      <c r="D125" s="39"/>
+      <c r="D125" s="37"/>
       <c r="E125" s="23"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
       <c r="A126" s="23"/>
       <c r="B126" s="23"/>
       <c r="C126" s="23"/>
-      <c r="D126" s="39"/>
+      <c r="D126" s="37"/>
       <c r="E126" s="23"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
       <c r="A127" s="23"/>
       <c r="B127" s="23"/>
       <c r="C127" s="23"/>
-      <c r="D127" s="39"/>
+      <c r="D127" s="37"/>
       <c r="E127" s="23"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
       <c r="A128" s="23"/>
       <c r="B128" s="23"/>
       <c r="C128" s="23"/>
-      <c r="D128" s="39"/>
+      <c r="D128" s="37"/>
       <c r="E128" s="23"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
       <c r="A129" s="23"/>
       <c r="B129" s="23"/>
       <c r="C129" s="23"/>
-      <c r="D129" s="39"/>
+      <c r="D129" s="37"/>
       <c r="E129" s="23"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
       <c r="A130" s="23"/>
       <c r="B130" s="23"/>
       <c r="C130" s="23"/>
-      <c r="D130" s="39"/>
+      <c r="D130" s="37"/>
       <c r="E130" s="23"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
       <c r="A131" s="23"/>
       <c r="B131" s="23"/>
       <c r="C131" s="23"/>
-      <c r="D131" s="39"/>
+      <c r="D131" s="37"/>
       <c r="E131" s="23"/>
     </row>
     <row r="132" ht="12.75" customHeight="1">
       <c r="A132" s="23"/>
       <c r="B132" s="23"/>
       <c r="C132" s="23"/>
-      <c r="D132" s="39"/>
+      <c r="D132" s="37"/>
       <c r="E132" s="23"/>
     </row>
     <row r="133" ht="12.75" customHeight="1">
       <c r="A133" s="23"/>
       <c r="B133" s="23"/>
       <c r="C133" s="23"/>
-      <c r="D133" s="39"/>
+      <c r="D133" s="37"/>
       <c r="E133" s="23"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
       <c r="A134" s="23"/>
       <c r="B134" s="23"/>
       <c r="C134" s="23"/>
-      <c r="D134" s="39"/>
+      <c r="D134" s="37"/>
       <c r="E134" s="23"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
       <c r="A135" s="23"/>
       <c r="B135" s="23"/>
       <c r="C135" s="23"/>
-      <c r="D135" s="39"/>
+      <c r="D135" s="37"/>
       <c r="E135" s="23"/>
     </row>
     <row r="136" ht="12.75" customHeight="1">
       <c r="A136" s="23"/>
       <c r="B136" s="23"/>
       <c r="C136" s="23"/>
-      <c r="D136" s="39"/>
+      <c r="D136" s="37"/>
       <c r="E136" s="23"/>
     </row>
     <row r="137" ht="12.75" customHeight="1">
       <c r="A137" s="23"/>
       <c r="B137" s="23"/>
       <c r="C137" s="23"/>
-      <c r="D137" s="39"/>
+      <c r="D137" s="37"/>
       <c r="E137" s="23"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
       <c r="A138" s="23"/>
       <c r="B138" s="23"/>
       <c r="C138" s="23"/>
-      <c r="D138" s="39"/>
+      <c r="D138" s="37"/>
       <c r="E138" s="23"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
       <c r="A139" s="23"/>
       <c r="B139" s="23"/>
       <c r="C139" s="23"/>
-      <c r="D139" s="39"/>
+      <c r="D139" s="37"/>
       <c r="E139" s="23"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
       <c r="A140" s="23"/>
       <c r="B140" s="23"/>
       <c r="C140" s="23"/>
-      <c r="D140" s="39"/>
+      <c r="D140" s="37"/>
       <c r="E140" s="23"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
       <c r="A141" s="23"/>
       <c r="B141" s="23"/>
       <c r="C141" s="23"/>
-      <c r="D141" s="39"/>
+      <c r="D141" s="37"/>
       <c r="E141" s="23"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
       <c r="A142" s="23"/>
       <c r="B142" s="23"/>
       <c r="C142" s="23"/>
-      <c r="D142" s="39"/>
+      <c r="D142" s="37"/>
       <c r="E142" s="23"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
       <c r="A143" s="23"/>
       <c r="B143" s="23"/>
       <c r="C143" s="23"/>
-      <c r="D143" s="39"/>
+      <c r="D143" s="37"/>
       <c r="E143" s="23"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
       <c r="A144" s="23"/>
       <c r="B144" s="23"/>
       <c r="C144" s="23"/>
-      <c r="D144" s="39"/>
+      <c r="D144" s="37"/>
       <c r="E144" s="23"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
       <c r="A145" s="23"/>
       <c r="B145" s="23"/>
       <c r="C145" s="23"/>
-      <c r="D145" s="39"/>
+      <c r="D145" s="37"/>
       <c r="E145" s="23"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
       <c r="A146" s="23"/>
       <c r="B146" s="23"/>
       <c r="C146" s="23"/>
-      <c r="D146" s="39"/>
+      <c r="D146" s="37"/>
       <c r="E146" s="23"/>
     </row>
     <row r="147" ht="12.75" customHeight="1">
       <c r="A147" s="23"/>
       <c r="B147" s="23"/>
       <c r="C147" s="23"/>
-      <c r="D147" s="39"/>
+      <c r="D147" s="37"/>
       <c r="E147" s="23"/>
     </row>
     <row r="148" ht="12.75" customHeight="1">
       <c r="A148" s="23"/>
       <c r="B148" s="23"/>
       <c r="C148" s="23"/>
-      <c r="D148" s="39"/>
+      <c r="D148" s="37"/>
       <c r="E148" s="23"/>
     </row>
     <row r="149" ht="12.75" customHeight="1">
       <c r="A149" s="23"/>
       <c r="B149" s="23"/>
       <c r="C149" s="23"/>
-      <c r="D149" s="39"/>
+      <c r="D149" s="37"/>
       <c r="E149" s="23"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
       <c r="A150" s="23"/>
       <c r="B150" s="23"/>
       <c r="C150" s="23"/>
-      <c r="D150" s="39"/>
+      <c r="D150" s="37"/>
       <c r="E150" s="23"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
       <c r="A151" s="23"/>
       <c r="B151" s="23"/>
       <c r="C151" s="23"/>
-      <c r="D151" s="39"/>
+      <c r="D151" s="37"/>
       <c r="E151" s="23"/>
     </row>
     <row r="152" ht="12.75" customHeight="1">
       <c r="A152" s="23"/>
       <c r="B152" s="23"/>
       <c r="C152" s="23"/>
-      <c r="D152" s="39"/>
+      <c r="D152" s="37"/>
       <c r="E152" s="23"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
       <c r="A153" s="23"/>
       <c r="B153" s="23"/>
       <c r="C153" s="23"/>
-      <c r="D153" s="39"/>
+      <c r="D153" s="37"/>
       <c r="E153" s="23"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
       <c r="A154" s="23"/>
       <c r="B154" s="23"/>
       <c r="C154" s="23"/>
-      <c r="D154" s="39"/>
+      <c r="D154" s="37"/>
       <c r="E154" s="23"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
       <c r="A155" s="23"/>
       <c r="B155" s="23"/>
       <c r="C155" s="23"/>
-      <c r="D155" s="39"/>
+      <c r="D155" s="37"/>
       <c r="E155" s="23"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
       <c r="A156" s="23"/>
       <c r="B156" s="23"/>
       <c r="C156" s="23"/>
-      <c r="D156" s="39"/>
+      <c r="D156" s="37"/>
       <c r="E156" s="23"/>
     </row>
     <row r="157" ht="12.75" customHeight="1">
       <c r="A157" s="23"/>
       <c r="B157" s="23"/>
       <c r="C157" s="23"/>
-      <c r="D157" s="39"/>
+      <c r="D157" s="37"/>
       <c r="E157" s="23"/>
     </row>
     <row r="158" ht="12.75" customHeight="1">
       <c r="A158" s="23"/>
       <c r="B158" s="23"/>
       <c r="C158" s="23"/>
-      <c r="D158" s="39"/>
+      <c r="D158" s="37"/>
       <c r="E158" s="23"/>
     </row>
     <row r="159" ht="12.75" customHeight="1">
       <c r="A159" s="23"/>
       <c r="B159" s="23"/>
       <c r="C159" s="23"/>
-      <c r="D159" s="39"/>
+      <c r="D159" s="37"/>
       <c r="E159" s="23"/>
     </row>
     <row r="160" ht="12.75" customHeight="1">
       <c r="A160" s="23"/>
       <c r="B160" s="23"/>
       <c r="C160" s="23"/>
-      <c r="D160" s="39"/>
+      <c r="D160" s="37"/>
       <c r="E160" s="23"/>
     </row>
     <row r="161" ht="12.75" customHeight="1">
       <c r="A161" s="23"/>
       <c r="B161" s="23"/>
       <c r="C161" s="23"/>
-      <c r="D161" s="39"/>
+      <c r="D161" s="37"/>
       <c r="E161" s="23"/>
     </row>
     <row r="162" ht="12.75" customHeight="1">
       <c r="A162" s="23"/>
       <c r="B162" s="23"/>
       <c r="C162" s="23"/>
-      <c r="D162" s="39"/>
+      <c r="D162" s="37"/>
       <c r="E162" s="23"/>
     </row>
     <row r="163" ht="12.75" customHeight="1">
       <c r="A163" s="23"/>
       <c r="B163" s="23"/>
       <c r="C163" s="23"/>
-      <c r="D163" s="39"/>
+      <c r="D163" s="37"/>
       <c r="E163" s="23"/>
     </row>
     <row r="164" ht="12.75" customHeight="1">
       <c r="A164" s="23"/>
       <c r="B164" s="23"/>
       <c r="C164" s="23"/>
-      <c r="D164" s="39"/>
+      <c r="D164" s="37"/>
       <c r="E164" s="23"/>
     </row>
     <row r="165" ht="12.75" customHeight="1">
       <c r="A165" s="23"/>
       <c r="B165" s="23"/>
       <c r="C165" s="23"/>
-      <c r="D165" s="39"/>
+      <c r="D165" s="37"/>
       <c r="E165" s="23"/>
     </row>
     <row r="166" ht="12.75" customHeight="1">
       <c r="A166" s="23"/>
       <c r="B166" s="23"/>
       <c r="C166" s="23"/>
-      <c r="D166" s="39"/>
+      <c r="D166" s="37"/>
       <c r="E166" s="23"/>
     </row>
     <row r="167" ht="12.75" customHeight="1">
       <c r="A167" s="23"/>
       <c r="B167" s="23"/>
       <c r="C167" s="23"/>
-      <c r="D167" s="39"/>
+      <c r="D167" s="37"/>
       <c r="E167" s="23"/>
     </row>
     <row r="168" ht="12.75" customHeight="1">
       <c r="A168" s="23"/>
       <c r="B168" s="23"/>
       <c r="C168" s="23"/>
-      <c r="D168" s="39"/>
+      <c r="D168" s="37"/>
       <c r="E168" s="23"/>
     </row>
     <row r="169" ht="12.75" customHeight="1">
       <c r="A169" s="23"/>
       <c r="B169" s="23"/>
       <c r="C169" s="23"/>
-      <c r="D169" s="39"/>
+      <c r="D169" s="37"/>
       <c r="E169" s="23"/>
     </row>
     <row r="170" ht="12.75" customHeight="1">
       <c r="A170" s="23"/>
       <c r="B170" s="23"/>
       <c r="C170" s="23"/>
-      <c r="D170" s="39"/>
+      <c r="D170" s="37"/>
       <c r="E170" s="23"/>
     </row>
     <row r="171" ht="12.75" customHeight="1">
       <c r="A171" s="23"/>
       <c r="B171" s="23"/>
       <c r="C171" s="23"/>
-      <c r="D171" s="39"/>
+      <c r="D171" s="37"/>
       <c r="E171" s="23"/>
     </row>
     <row r="172" ht="12.75" customHeight="1">
       <c r="A172" s="23"/>
       <c r="B172" s="23"/>
       <c r="C172" s="23"/>
-      <c r="D172" s="39"/>
+      <c r="D172" s="37"/>
       <c r="E172" s="23"/>
     </row>
     <row r="173" ht="12.75" customHeight="1">
       <c r="A173" s="23"/>
       <c r="B173" s="23"/>
       <c r="C173" s="23"/>
-      <c r="D173" s="39"/>
+      <c r="D173" s="37"/>
       <c r="E173" s="23"/>
     </row>
     <row r="174" ht="12.75" customHeight="1">
       <c r="A174" s="23"/>
       <c r="B174" s="23"/>
       <c r="C174" s="23"/>
-      <c r="D174" s="39"/>
+      <c r="D174" s="37"/>
       <c r="E174" s="23"/>
     </row>
     <row r="175" ht="12.75" customHeight="1">
       <c r="A175" s="23"/>
       <c r="B175" s="23"/>
       <c r="C175" s="23"/>
-      <c r="D175" s="39"/>
+      <c r="D175" s="37"/>
       <c r="E175" s="23"/>
     </row>
     <row r="176" ht="12.75" customHeight="1">
       <c r="A176" s="23"/>
       <c r="B176" s="23"/>
       <c r="C176" s="23"/>
-      <c r="D176" s="39"/>
+      <c r="D176" s="37"/>
       <c r="E176" s="23"/>
     </row>
     <row r="177" ht="12.75" customHeight="1">
       <c r="A177" s="23"/>
       <c r="B177" s="23"/>
       <c r="C177" s="23"/>
-      <c r="D177" s="39"/>
+      <c r="D177" s="37"/>
       <c r="E177" s="23"/>
     </row>
     <row r="178" ht="12.75" customHeight="1">
       <c r="A178" s="23"/>
       <c r="B178" s="23"/>
       <c r="C178" s="23"/>
-      <c r="D178" s="39"/>
+      <c r="D178" s="37"/>
       <c r="E178" s="23"/>
     </row>
     <row r="179" ht="12.75" customHeight="1">
       <c r="A179" s="23"/>
       <c r="B179" s="23"/>
       <c r="C179" s="23"/>
-      <c r="D179" s="39"/>
+      <c r="D179" s="37"/>
       <c r="E179" s="23"/>
     </row>
     <row r="180" ht="12.75" customHeight="1">
       <c r="A180" s="23"/>
       <c r="B180" s="23"/>
       <c r="C180" s="23"/>
-      <c r="D180" s="39"/>
+      <c r="D180" s="37"/>
       <c r="E180" s="23"/>
     </row>
     <row r="181" ht="12.75" customHeight="1">
       <c r="A181" s="23"/>
       <c r="B181" s="23"/>
       <c r="C181" s="23"/>
-      <c r="D181" s="39"/>
+      <c r="D181" s="37"/>
       <c r="E181" s="23"/>
     </row>
     <row r="182" ht="12.75" customHeight="1">
       <c r="A182" s="23"/>
       <c r="B182" s="23"/>
       <c r="C182" s="23"/>
-      <c r="D182" s="39"/>
+      <c r="D182" s="37"/>
       <c r="E182" s="23"/>
     </row>
     <row r="183" ht="12.75" customHeight="1">
       <c r="A183" s="23"/>
       <c r="B183" s="23"/>
       <c r="C183" s="23"/>
-      <c r="D183" s="39"/>
+      <c r="D183" s="37"/>
       <c r="E183" s="23"/>
     </row>
     <row r="184" ht="12.75" customHeight="1">
       <c r="A184" s="23"/>
       <c r="B184" s="23"/>
       <c r="C184" s="23"/>
-      <c r="D184" s="39"/>
+      <c r="D184" s="37"/>
       <c r="E184" s="23"/>
     </row>
     <row r="185" ht="12.75" customHeight="1">
       <c r="A185" s="23"/>
       <c r="B185" s="23"/>
       <c r="C185" s="23"/>
-      <c r="D185" s="39"/>
+      <c r="D185" s="37"/>
       <c r="E185" s="23"/>
     </row>
     <row r="186" ht="12.75" customHeight="1">
       <c r="A186" s="23"/>
       <c r="B186" s="23"/>
       <c r="C186" s="23"/>
-      <c r="D186" s="39"/>
+      <c r="D186" s="37"/>
       <c r="E186" s="23"/>
     </row>
     <row r="187" ht="12.75" customHeight="1">
       <c r="A187" s="23"/>
       <c r="B187" s="23"/>
       <c r="C187" s="23"/>
-      <c r="D187" s="39"/>
+      <c r="D187" s="37"/>
       <c r="E187" s="23"/>
     </row>
     <row r="188" ht="12.75" customHeight="1">
       <c r="A188" s="23"/>
       <c r="B188" s="23"/>
       <c r="C188" s="23"/>
-      <c r="D188" s="39"/>
+      <c r="D188" s="37"/>
       <c r="E188" s="23"/>
     </row>
     <row r="189" ht="12.75" customHeight="1">
       <c r="A189" s="23"/>
       <c r="B189" s="23"/>
       <c r="C189" s="23"/>
-      <c r="D189" s="39"/>
+      <c r="D189" s="37"/>
       <c r="E189" s="23"/>
     </row>
     <row r="190" ht="12.75" customHeight="1">
       <c r="A190" s="23"/>
       <c r="B190" s="23"/>
       <c r="C190" s="23"/>
-      <c r="D190" s="39"/>
+      <c r="D190" s="37"/>
       <c r="E190" s="23"/>
     </row>
     <row r="191" ht="12.75" customHeight="1">
       <c r="A191" s="23"/>
       <c r="B191" s="23"/>
       <c r="C191" s="23"/>
-      <c r="D191" s="39"/>
+      <c r="D191" s="37"/>
       <c r="E191" s="23"/>
     </row>
     <row r="192" ht="12.75" customHeight="1">
       <c r="A192" s="23"/>
       <c r="B192" s="23"/>
       <c r="C192" s="23"/>
-      <c r="D192" s="39"/>
+      <c r="D192" s="37"/>
       <c r="E192" s="23"/>
     </row>
     <row r="193" ht="12.75" customHeight="1">
       <c r="A193" s="23"/>
       <c r="B193" s="23"/>
       <c r="C193" s="23"/>
-      <c r="D193" s="39"/>
+      <c r="D193" s="37"/>
       <c r="E193" s="23"/>
     </row>
     <row r="194" ht="12.75" customHeight="1">
       <c r="A194" s="23"/>
       <c r="B194" s="23"/>
       <c r="C194" s="23"/>
-      <c r="D194" s="39"/>
+      <c r="D194" s="37"/>
       <c r="E194" s="23"/>
     </row>
     <row r="195" ht="12.75" customHeight="1">
       <c r="A195" s="23"/>
       <c r="B195" s="23"/>
       <c r="C195" s="23"/>
-      <c r="D195" s="39"/>
+      <c r="D195" s="37"/>
       <c r="E195" s="23"/>
     </row>
     <row r="196" ht="12.75" customHeight="1">
       <c r="A196" s="23"/>
       <c r="B196" s="23"/>
       <c r="C196" s="23"/>
-      <c r="D196" s="39"/>
+      <c r="D196" s="37"/>
       <c r="E196" s="23"/>
     </row>
     <row r="197" ht="12.75" customHeight="1">
       <c r="A197" s="23"/>
       <c r="B197" s="23"/>
       <c r="C197" s="23"/>
-      <c r="D197" s="39"/>
+      <c r="D197" s="37"/>
       <c r="E197" s="23"/>
     </row>
     <row r="198" ht="12.75" customHeight="1">
       <c r="A198" s="23"/>
       <c r="B198" s="23"/>
       <c r="C198" s="23"/>
-      <c r="D198" s="39"/>
+      <c r="D198" s="37"/>
       <c r="E198" s="23"/>
     </row>
     <row r="199" ht="12.75" customHeight="1">
       <c r="A199" s="23"/>
       <c r="B199" s="23"/>
       <c r="C199" s="23"/>
-      <c r="D199" s="39"/>
+      <c r="D199" s="37"/>
       <c r="E199" s="23"/>
     </row>
     <row r="200" ht="12.75" customHeight="1">
       <c r="A200" s="23"/>
       <c r="B200" s="23"/>
       <c r="C200" s="23"/>
-      <c r="D200" s="39"/>
+      <c r="D200" s="37"/>
       <c r="E200" s="23"/>
     </row>
     <row r="201" ht="12.75" customHeight="1">
       <c r="A201" s="23"/>
       <c r="B201" s="23"/>
       <c r="C201" s="23"/>
-      <c r="D201" s="39"/>
+      <c r="D201" s="37"/>
       <c r="E201" s="23"/>
     </row>
     <row r="202" ht="12.75" customHeight="1">
       <c r="A202" s="23"/>
       <c r="B202" s="23"/>
       <c r="C202" s="23"/>
-      <c r="D202" s="39"/>
+      <c r="D202" s="37"/>
       <c r="E202" s="23"/>
     </row>
     <row r="203" ht="12.75" customHeight="1">
       <c r="A203" s="23"/>
       <c r="B203" s="23"/>
       <c r="C203" s="23"/>
-      <c r="D203" s="39"/>
+      <c r="D203" s="37"/>
       <c r="E203" s="23"/>
     </row>
     <row r="204" ht="12.75" customHeight="1">
       <c r="A204" s="23"/>
       <c r="B204" s="23"/>
       <c r="C204" s="23"/>
-      <c r="D204" s="39"/>
+      <c r="D204" s="37"/>
       <c r="E204" s="23"/>
     </row>
     <row r="205" ht="12.75" customHeight="1">
       <c r="A205" s="23"/>
       <c r="B205" s="23"/>
       <c r="C205" s="23"/>
-      <c r="D205" s="39"/>
+      <c r="D205" s="37"/>
       <c r="E205" s="23"/>
     </row>
     <row r="206" ht="12.75" customHeight="1">
       <c r="A206" s="23"/>
       <c r="B206" s="23"/>
       <c r="C206" s="23"/>
-      <c r="D206" s="39"/>
+      <c r="D206" s="37"/>
       <c r="E206" s="23"/>
     </row>
     <row r="207" ht="12.75" customHeight="1">
       <c r="A207" s="23"/>
       <c r="B207" s="23"/>
       <c r="C207" s="23"/>
-      <c r="D207" s="39"/>
+      <c r="D207" s="37"/>
       <c r="E207" s="23"/>
     </row>
     <row r="208" ht="12.75" customHeight="1">
       <c r="A208" s="23"/>
       <c r="B208" s="23"/>
       <c r="C208" s="23"/>
-      <c r="D208" s="39"/>
+      <c r="D208" s="37"/>
       <c r="E208" s="23"/>
     </row>
     <row r="209" ht="12.75" customHeight="1">
       <c r="A209" s="23"/>
       <c r="B209" s="23"/>
       <c r="C209" s="23"/>
-      <c r="D209" s="39"/>
+      <c r="D209" s="37"/>
       <c r="E209" s="23"/>
     </row>
     <row r="210" ht="12.75" customHeight="1">
       <c r="A210" s="23"/>
       <c r="B210" s="23"/>
       <c r="C210" s="23"/>
-      <c r="D210" s="39"/>
+      <c r="D210" s="37"/>
       <c r="E210" s="23"/>
     </row>
     <row r="211" ht="12.75" customHeight="1">
       <c r="A211" s="23"/>
       <c r="B211" s="23"/>
       <c r="C211" s="23"/>
-      <c r="D211" s="39"/>
+      <c r="D211" s="37"/>
       <c r="E211" s="23"/>
     </row>
     <row r="212" ht="12.75" customHeight="1">
       <c r="A212" s="23"/>
       <c r="B212" s="23"/>
       <c r="C212" s="23"/>
-      <c r="D212" s="39"/>
+      <c r="D212" s="37"/>
       <c r="E212" s="23"/>
     </row>
     <row r="213" ht="12.75" customHeight="1">
       <c r="A213" s="23"/>
       <c r="B213" s="23"/>
       <c r="C213" s="23"/>
-      <c r="D213" s="39"/>
+      <c r="D213" s="37"/>
       <c r="E213" s="23"/>
     </row>
     <row r="214" ht="12.75" customHeight="1">
       <c r="A214" s="23"/>
       <c r="B214" s="23"/>
       <c r="C214" s="23"/>
-      <c r="D214" s="39"/>
+      <c r="D214" s="37"/>
       <c r="E214" s="23"/>
     </row>
     <row r="215" ht="12.75" customHeight="1">
       <c r="A215" s="23"/>
       <c r="B215" s="23"/>
       <c r="C215" s="23"/>
-      <c r="D215" s="39"/>
+      <c r="D215" s="37"/>
       <c r="E215" s="23"/>
     </row>
     <row r="216" ht="12.75" customHeight="1">
       <c r="A216" s="23"/>
       <c r="B216" s="23"/>
       <c r="C216" s="23"/>
-      <c r="D216" s="39"/>
+      <c r="D216" s="37"/>
       <c r="E216" s="23"/>
     </row>
     <row r="217" ht="12.75" customHeight="1">
       <c r="A217" s="23"/>
       <c r="B217" s="23"/>
       <c r="C217" s="23"/>
-      <c r="D217" s="39"/>
+      <c r="D217" s="37"/>
       <c r="E217" s="23"/>
     </row>
     <row r="218" ht="12.75" customHeight="1"/>
@@ -12666,404 +12692,404 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="70" t="s">
-        <v>217</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>218</v>
-      </c>
-      <c r="C1" s="70" t="s">
-        <v>219</v>
+      <c r="A1" s="67" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>221</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>222</v>
+      <c r="A2" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>224</v>
+      <c r="A3" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="37" t="s">
-        <v>225</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>227</v>
+      <c r="A4" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="37" t="s">
-        <v>228</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" s="37" t="s">
-        <v>230</v>
+      <c r="A5" s="36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="37" t="s">
-        <v>231</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="C6" s="37" t="s">
-        <v>233</v>
+      <c r="A6" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="B6" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>236</v>
+      <c r="A7" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="37" t="s">
-        <v>237</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>239</v>
+      <c r="A8" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>242</v>
+      <c r="A9" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>244</v>
-      </c>
-      <c r="C10" s="37" t="s">
-        <v>245</v>
+      <c r="A10" s="36" t="s">
+        <v>246</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="37" t="s">
-        <v>246</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="C11" s="37" t="s">
-        <v>248</v>
+      <c r="A11" s="36" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>250</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>251</v>
+      <c r="A12" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>254</v>
+      <c r="A13" s="36" t="s">
+        <v>255</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" s="36" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="37"/>
-      <c r="B14" s="37" t="s">
-        <v>255</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>256</v>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37" t="s">
-        <v>257</v>
-      </c>
-      <c r="C15" s="37" t="s">
-        <v>258</v>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37" t="s">
-        <v>259</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>260</v>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="37"/>
-      <c r="B17" s="37" t="s">
-        <v>261</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>262</v>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="37"/>
-      <c r="B18" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>264</v>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="37"/>
-      <c r="B19" s="37" t="s">
-        <v>265</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>266</v>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>269</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37" t="s">
-        <v>267</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>268</v>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="37"/>
-      <c r="B21" s="37" t="s">
-        <v>269</v>
-      </c>
-      <c r="C21" s="37" t="s">
-        <v>270</v>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="37"/>
-      <c r="B22" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>272</v>
+      <c r="A22" s="36"/>
+      <c r="B22" s="36" t="s">
+        <v>274</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="37"/>
-      <c r="B23" s="37" t="s">
-        <v>273</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>274</v>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="37"/>
-      <c r="B24" s="37" t="s">
-        <v>275</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>276</v>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36" t="s">
+        <v>278</v>
+      </c>
+      <c r="C24" s="36" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="37"/>
-      <c r="B25" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>278</v>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36" t="s">
+        <v>280</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="37"/>
-      <c r="B26" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>280</v>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" s="36" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="37"/>
-      <c r="B27" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="C27" s="37"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="C27" s="36"/>
     </row>
     <row r="28">
-      <c r="A28" s="37"/>
-      <c r="B28" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="C28" s="37"/>
+      <c r="A28" s="36"/>
+      <c r="B28" s="36" t="s">
+        <v>285</v>
+      </c>
+      <c r="C28" s="36"/>
     </row>
     <row r="29">
-      <c r="A29" s="37"/>
-      <c r="B29" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="C29" s="37"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36" t="s">
+        <v>286</v>
+      </c>
+      <c r="C29" s="36"/>
     </row>
     <row r="30">
-      <c r="A30" s="37"/>
-      <c r="B30" s="37" t="s">
-        <v>284</v>
-      </c>
-      <c r="C30" s="37"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C30" s="36"/>
     </row>
     <row r="31">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="C31" s="37"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36" t="s">
+        <v>288</v>
+      </c>
+      <c r="C31" s="36"/>
     </row>
     <row r="32">
-      <c r="A32" s="37"/>
-      <c r="B32" s="37" t="s">
-        <v>286</v>
-      </c>
-      <c r="C32" s="37"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36" t="s">
+        <v>289</v>
+      </c>
+      <c r="C32" s="36"/>
     </row>
     <row r="33">
-      <c r="A33" s="37"/>
-      <c r="B33" s="37" t="s">
-        <v>287</v>
-      </c>
-      <c r="C33" s="37"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36" t="s">
+        <v>290</v>
+      </c>
+      <c r="C33" s="36"/>
     </row>
     <row r="34">
-      <c r="A34" s="37"/>
-      <c r="B34" s="37" t="s">
-        <v>288</v>
-      </c>
-      <c r="C34" s="37"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="C34" s="36"/>
     </row>
     <row r="35">
-      <c r="A35" s="37"/>
-      <c r="B35" s="37" t="s">
-        <v>289</v>
-      </c>
-      <c r="C35" s="37"/>
+      <c r="A35" s="36"/>
+      <c r="B35" s="36" t="s">
+        <v>292</v>
+      </c>
+      <c r="C35" s="36"/>
     </row>
     <row r="36">
-      <c r="A36" s="37"/>
-      <c r="B36" s="37" t="s">
-        <v>290</v>
-      </c>
-      <c r="C36" s="37"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36" t="s">
+        <v>293</v>
+      </c>
+      <c r="C36" s="36"/>
     </row>
     <row r="37">
-      <c r="A37" s="37"/>
-      <c r="B37" s="37" t="s">
-        <v>291</v>
-      </c>
-      <c r="C37" s="37"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="C37" s="36"/>
     </row>
     <row r="38">
-      <c r="A38" s="37"/>
-      <c r="B38" s="37" t="s">
-        <v>292</v>
-      </c>
-      <c r="C38" s="37"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C38" s="36"/>
     </row>
     <row r="39">
-      <c r="A39" s="37"/>
-      <c r="B39" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="C39" s="37"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36" t="s">
+        <v>296</v>
+      </c>
+      <c r="C39" s="36"/>
     </row>
     <row r="40">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37" t="s">
-        <v>294</v>
-      </c>
-      <c r="C40" s="37"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40" s="36"/>
     </row>
     <row r="41">
-      <c r="A41" s="37"/>
-      <c r="B41" s="37" t="s">
-        <v>295</v>
-      </c>
-      <c r="C41" s="37"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C41" s="36"/>
     </row>
     <row r="42">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37" t="s">
-        <v>296</v>
-      </c>
-      <c r="C42" s="37"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36" t="s">
+        <v>299</v>
+      </c>
+      <c r="C42" s="36"/>
     </row>
     <row r="43">
-      <c r="A43" s="37"/>
-      <c r="B43" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="C43" s="37"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="C43" s="36"/>
     </row>
     <row r="44">
-      <c r="A44" s="37"/>
-      <c r="B44" s="37" t="s">
-        <v>298</v>
-      </c>
-      <c r="C44" s="37"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="C44" s="36"/>
     </row>
     <row r="45">
-      <c r="A45" s="37"/>
-      <c r="B45" s="37" t="s">
-        <v>299</v>
-      </c>
-      <c r="C45" s="37"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="C45" s="36"/>
     </row>
     <row r="46">
-      <c r="A46" s="37"/>
-      <c r="B46" s="37" t="s">
-        <v>300</v>
-      </c>
-      <c r="C46" s="37"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36" t="s">
+        <v>303</v>
+      </c>
+      <c r="C46" s="36"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Fix PersonneEtOrganization in hierarchical config
</commit_message>
<xml_diff>
--- a/dev-page/configs/sparnatural-hierarchy-config.xlsx
+++ b/dev-page/configs/sparnatural-hierarchy-config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Prefixes" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <si>
     <r>
       <rPr>
@@ -697,6 +697,24 @@
     <t xml:space="preserve">exerce dans le quartier ou la voie</t>
   </si>
   <si>
+    <t xml:space="preserve">(rico:agentIsTargetOfPerformanceRelation rico:beginningDate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has beginning date of occupation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a pour date de début d'exercice</t>
+  </si>
+  <si>
+    <t>sh:Literal</t>
+  </si>
+  <si>
+    <t>xsd:date</t>
+  </si>
+  <si>
+    <t>core:TimeProperty-Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">URI of the datasource in the configuration. This is the value that should be referenced from the "datasources:datasource" column in the properties tab</t>
   </si>
   <si>
@@ -818,9 +836,6 @@
   </si>
   <si>
     <t>datasources:query_list_label_count</t>
-  </si>
-  <si>
-    <t>core:TimeProperty-Date</t>
   </si>
   <si>
     <t>datasources:list_dctermstitle_alpha_with_count</t>
@@ -1313,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1397,9 +1412,6 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf fontId="12" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3814,7 +3826,7 @@
       <c r="L20" s="34"/>
       <c r="M20" s="38"/>
       <c r="N20" s="33"/>
-      <c r="O20" s="39" t="s">
+      <c r="O20" s="33" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3831,9 +3843,7 @@
       <c r="D21" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="29" t="s">
-        <v>119</v>
-      </c>
+      <c r="E21" s="29"/>
       <c r="F21" s="29" t="s">
         <v>66</v>
       </c>
@@ -3849,7 +3859,7 @@
       <c r="L21" s="34"/>
       <c r="M21" s="38"/>
       <c r="N21" s="33"/>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="33" t="s">
         <v>137</v>
       </c>
     </row>
@@ -6431,7 +6441,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
@@ -6462,21 +6472,21 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="41" t="str">
+      <c r="B1" s="40" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
       <c r="F1" s="36"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="44"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
       <c r="K1" s="23"/>
       <c r="L1" s="23"/>
       <c r="M1" s="23"/>
@@ -6488,11 +6498,11 @@
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="17"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
       <c r="K2" s="23"/>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -6504,11 +6514,11 @@
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="17"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
       <c r="M3" s="23"/>
@@ -6523,8 +6533,8 @@
       <c r="D4" s="36"/>
       <c r="E4" s="36"/>
       <c r="F4" s="36"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23"/>
@@ -6694,53 +6704,53 @@
       <c r="X7" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="Y7" s="46"/>
-      <c r="Z7" s="46"/>
-      <c r="AA7" s="46"/>
-      <c r="AB7" s="46"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="45"/>
+      <c r="AA7" s="45"/>
+      <c r="AB7" s="45"/>
     </row>
     <row r="8" ht="15.75">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Y8" s="48"/>
-      <c r="Z8" s="48"/>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="48"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
+      <c r="N8" s="47"/>
+      <c r="O8" s="47"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="47"/>
+      <c r="R8" s="47"/>
+      <c r="S8" s="47"/>
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="V8" s="47"/>
+      <c r="W8" s="47"/>
+      <c r="X8" s="47"/>
+      <c r="Y8" s="47"/>
+      <c r="Z8" s="47"/>
+      <c r="AA8" s="47"/>
+      <c r="AB8" s="47"/>
+      <c r="AC8" s="47"/>
     </row>
     <row r="9" ht="25.5">
-      <c r="A9" s="50" t="str">
+      <c r="A9" s="49" t="str">
         <f>CONCATENATE("this:",RIGHT(C9,LEN(C9)-SEARCH(":",C9)),"_",RIGHT(B9,LEN(B9)-SEARCH(":",B9)))</f>
         <v>this:Place_hasOrHadPlaceType</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="51" t="s">
         <v>182</v>
       </c>
       <c r="D9" s="7">
@@ -6753,20 +6763,20 @@
       <c r="F9" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50">
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49">
         <v>1</v>
       </c>
-      <c r="K9" s="50" t="s">
+      <c r="K9" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50" t="s">
+      <c r="L9" s="49"/>
+      <c r="M9" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="N9" s="50"/>
+      <c r="N9" s="49"/>
       <c r="O9" s="30" t="s">
         <v>185</v>
       </c>
@@ -6788,17 +6798,17 @@
       <c r="AC9" s="34"/>
     </row>
     <row r="10" ht="14.25">
-      <c r="A10" s="50"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="31"/>
-      <c r="C10" s="52"/>
+      <c r="C10" s="51"/>
       <c r="D10" s="34"/>
       <c r="E10" s="30"/>
       <c r="F10" s="30"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
       <c r="L10" s="34"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -6819,17 +6829,17 @@
       <c r="AC10" s="34"/>
     </row>
     <row r="11" ht="14.25">
-      <c r="A11" s="50"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="33"/>
-      <c r="C11" s="52"/>
+      <c r="C11" s="51"/>
       <c r="D11" s="34"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
       <c r="G11" s="31"/>
-      <c r="H11" s="53"/>
+      <c r="H11" s="52"/>
       <c r="I11" s="34"/>
       <c r="J11" s="34"/>
-      <c r="K11" s="50"/>
+      <c r="K11" s="49"/>
       <c r="L11" s="34"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -6850,17 +6860,17 @@
       <c r="AC11" s="34"/>
     </row>
     <row r="12" ht="14.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="31"/>
-      <c r="C12" s="52"/>
+      <c r="C12" s="51"/>
       <c r="D12" s="34"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
-      <c r="H12" s="53"/>
+      <c r="H12" s="52"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
-      <c r="K12" s="50"/>
+      <c r="K12" s="49"/>
       <c r="L12" s="34"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
@@ -6881,51 +6891,51 @@
       <c r="AC12" s="34"/>
     </row>
     <row r="13" ht="15.75">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="48"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="48"/>
-      <c r="X13" s="48"/>
-      <c r="Y13" s="48"/>
-      <c r="Z13" s="48"/>
-      <c r="AA13" s="48"/>
-      <c r="AB13" s="48"/>
-      <c r="AC13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="47"/>
+      <c r="W13" s="47"/>
+      <c r="X13" s="47"/>
+      <c r="Y13" s="47"/>
+      <c r="Z13" s="47"/>
+      <c r="AA13" s="47"/>
+      <c r="AB13" s="47"/>
+      <c r="AC13" s="47"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="A14" s="50"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="53"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="34"/>
       <c r="E14" s="30"/>
       <c r="F14" s="30"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
       <c r="I14" s="34"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
-      <c r="L14" s="50"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="30"/>
@@ -6945,47 +6955,47 @@
       <c r="AC14" s="34"/>
     </row>
     <row r="15" ht="15.75">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="46" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="48"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="48"/>
-      <c r="X15" s="48"/>
-      <c r="Y15" s="48"/>
-      <c r="Z15" s="48"/>
-      <c r="AA15" s="48"/>
-      <c r="AB15" s="48"/>
-      <c r="AC15" s="48"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="47"/>
+      <c r="J15" s="47"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="47"/>
+      <c r="O15" s="47"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="47"/>
+      <c r="X15" s="47"/>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
+      <c r="AB15" s="47"/>
+      <c r="AC15" s="47"/>
     </row>
     <row r="16" ht="14.25">
-      <c r="A16" s="50"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="31"/>
-      <c r="C16" s="53"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="34"/>
       <c r="E16" s="30"/>
       <c r="F16" s="30"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
@@ -7009,14 +7019,14 @@
       <c r="AC16" s="34"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="A17" s="50"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="31"/>
-      <c r="C17" s="53"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="34"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
@@ -7039,14 +7049,14 @@
       <c r="AC17" s="34"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="A18" s="50"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="31"/>
-      <c r="C18" s="53"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="34"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
       <c r="I18" s="34"/>
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
@@ -7069,14 +7079,14 @@
       <c r="AC18" s="34"/>
     </row>
     <row r="19" ht="14.25">
-      <c r="A19" s="50"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="31"/>
-      <c r="C19" s="53"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="34"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="31"/>
-      <c r="H19" s="53"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="34"/>
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
@@ -7098,14 +7108,14 @@
       <c r="AC19" s="34"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="A20" s="50"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="31"/>
-      <c r="C20" s="53"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="34"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="53"/>
+      <c r="H20" s="52"/>
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="34"/>
@@ -7129,40 +7139,40 @@
       <c r="AC20" s="34"/>
     </row>
     <row r="21" ht="15.75">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="46" t="s">
         <v>189</v>
       </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="48"/>
-      <c r="N21" s="48"/>
-      <c r="O21" s="48"/>
-      <c r="P21" s="48"/>
-      <c r="Q21" s="48"/>
-      <c r="R21" s="48"/>
-      <c r="S21" s="48"/>
-      <c r="T21" s="48"/>
-      <c r="U21" s="48"/>
-      <c r="V21" s="48"/>
-      <c r="W21" s="48"/>
-      <c r="X21" s="48"/>
-      <c r="Y21" s="48"/>
-      <c r="Z21" s="48"/>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="48"/>
-      <c r="AC21" s="48"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="A22" s="50"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="34"/>
@@ -7174,8 +7184,8 @@
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
       <c r="L22" s="34"/>
-      <c r="M22" s="50"/>
-      <c r="N22" s="50"/>
+      <c r="M22" s="49"/>
+      <c r="N22" s="49"/>
       <c r="O22" s="34"/>
       <c r="P22" s="34"/>
       <c r="Q22" s="34"/>
@@ -7193,7 +7203,7 @@
       <c r="AC22" s="34"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="A23" s="50"/>
+      <c r="A23" s="49"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="34"/>
@@ -7223,47 +7233,47 @@
       <c r="AC23" s="34"/>
     </row>
     <row r="24" ht="15.75">
-      <c r="A24" s="47" t="s">
+      <c r="A24" s="46" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="49"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="48"/>
-      <c r="Z24" s="48"/>
-      <c r="AA24" s="48"/>
-      <c r="AB24" s="48"/>
-      <c r="AC24" s="48"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
+      <c r="L24" s="47"/>
+      <c r="M24" s="47"/>
+      <c r="N24" s="47"/>
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="V24" s="47"/>
+      <c r="W24" s="47"/>
+      <c r="X24" s="47"/>
+      <c r="Y24" s="47"/>
+      <c r="Z24" s="47"/>
+      <c r="AA24" s="47"/>
+      <c r="AB24" s="47"/>
+      <c r="AC24" s="47"/>
     </row>
     <row r="25" ht="15">
-      <c r="A25" s="50" t="str">
+      <c r="A25" s="49" t="str">
         <f>CONCATENATE("this:",RIGHT(C25,LEN(C25)-SEARCH(":",C25)),"_",RIGHT(B25,LEN(B25)-SEARCH(":",B25)))</f>
         <v>this:Adresse_hasOrHadLocation</v>
       </c>
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="C25" s="52" t="s">
+      <c r="C25" s="51" t="s">
         <v>97</v>
       </c>
       <c r="D25" s="7">
@@ -7276,16 +7286,16 @@
       <c r="F25" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="G25" s="53"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="50" t="s">
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="L25" s="50"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="50" t="s">
+      <c r="L25" s="49"/>
+      <c r="M25" s="49"/>
+      <c r="N25" s="49" t="s">
         <v>193</v>
       </c>
       <c r="O25" s="30" t="s">
@@ -7311,13 +7321,13 @@
       <c r="AC25" s="34"/>
     </row>
     <row r="26" ht="28.5">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="53" t="s">
         <v>195</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="50" t="s">
         <v>196</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="51" t="s">
         <v>97</v>
       </c>
       <c r="D26" s="7">
@@ -7330,16 +7340,16 @@
       <c r="F26" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="50" t="s">
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="L26" s="50"/>
-      <c r="M26" s="50"/>
-      <c r="N26" s="50" t="s">
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49" t="s">
         <v>199</v>
       </c>
       <c r="O26" s="30" t="s">
@@ -7371,46 +7381,46 @@
       <c r="O27" s="7"/>
     </row>
     <row r="28" ht="15.75">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="48"/>
-      <c r="M28" s="48"/>
-      <c r="N28" s="48"/>
-      <c r="O28" s="48"/>
-      <c r="P28" s="48"/>
-      <c r="Q28" s="48"/>
-      <c r="R28" s="48"/>
-      <c r="S28" s="48"/>
-      <c r="T28" s="48"/>
-      <c r="U28" s="48"/>
-      <c r="V28" s="48"/>
-      <c r="W28" s="48"/>
-      <c r="X28" s="48"/>
-      <c r="Y28" s="48"/>
-      <c r="Z28" s="48"/>
-      <c r="AA28" s="48"/>
-      <c r="AB28" s="48"/>
-      <c r="AC28" s="48"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="48"/>
+      <c r="I28" s="47"/>
+      <c r="J28" s="47"/>
+      <c r="K28" s="47"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="47"/>
+      <c r="O28" s="47"/>
+      <c r="P28" s="47"/>
+      <c r="Q28" s="47"/>
+      <c r="R28" s="47"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="47"/>
+      <c r="V28" s="47"/>
+      <c r="W28" s="47"/>
+      <c r="X28" s="47"/>
+      <c r="Y28" s="47"/>
+      <c r="Z28" s="47"/>
+      <c r="AA28" s="47"/>
+      <c r="AB28" s="47"/>
+      <c r="AC28" s="47"/>
     </row>
     <row r="29" ht="28.5">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="53" t="s">
         <v>201</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="C29" s="52" t="s">
+      <c r="C29" s="51" t="s">
         <v>203</v>
       </c>
       <c r="D29" s="7">
@@ -7423,16 +7433,16 @@
       <c r="F29" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50" t="s">
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="L29" s="50"/>
-      <c r="M29" s="50"/>
-      <c r="N29" s="50" t="s">
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49" t="s">
         <v>193</v>
       </c>
       <c r="O29" s="30" t="s">
@@ -7464,16 +7474,66 @@
       <c r="O30" s="7"/>
     </row>
     <row r="31" ht="15">
-      <c r="C31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="O31" s="7"/>
+      <c r="A31" s="46" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="47"/>
+      <c r="P31" s="47"/>
+      <c r="Q31" s="47"/>
+      <c r="R31" s="47"/>
+      <c r="S31" s="47"/>
+      <c r="T31" s="47"/>
+      <c r="U31" s="47"/>
+      <c r="V31" s="47"/>
+      <c r="W31" s="47"/>
+      <c r="X31" s="47"/>
+      <c r="Y31" s="47"/>
+      <c r="Z31" s="47"/>
+      <c r="AA31" s="47"/>
+      <c r="AB31" s="47"/>
+      <c r="AC31" s="47"/>
     </row>
     <row r="32" ht="15">
-      <c r="C32" s="17"/>
+      <c r="A32" s="49" t="str">
+        <f>CONCATENATE("this:",RIGHT(C32,LEN(C32)-SEARCH(":",C32)),"_",RIGHT(B32,LEN(B32)-SEARCH(":",B32)))</f>
+        <v xml:space="preserve">this:Personne, this:Organization_agentIsTargetOfPerformanceRelation rico:beginningDate)</v>
+      </c>
+      <c r="B32" s="50" t="s">
+        <v>206</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" t="s">
+        <v>207</v>
+      </c>
+      <c r="F32" t="s">
+        <v>208</v>
+      </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
-      <c r="O32" s="7"/>
+      <c r="K32" t="s">
+        <v>209</v>
+      </c>
+      <c r="L32" t="s">
+        <v>210</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="33" ht="15">
       <c r="C33" s="17"/>
@@ -9001,7 +9061,7 @@
     <row r="947" ht="15"/>
   </sheetData>
   <dataValidations count="14" disablePrompts="0">
-    <dataValidation sqref="O27 O30:O45" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+    <dataValidation sqref="O27 O30 O32:O45" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>'sparnatural-config-core'!$A$2:$A$13</formula1>
     </dataValidation>
     <dataValidation sqref="O9" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
@@ -9078,18 +9138,18 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="56" t="str">
+      <c r="B1" s="55" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="23"/>
-      <c r="E1" s="57"/>
+      <c r="E1" s="56"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -9107,66 +9167,66 @@
       <c r="I2" s="23"/>
     </row>
     <row r="3" ht="91.5" customHeight="1">
-      <c r="A3" s="58" t="s">
-        <v>206</v>
-      </c>
-      <c r="B3" s="58" t="s">
-        <v>207</v>
-      </c>
-      <c r="C3" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>210</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>211</v>
+      <c r="A3" s="57" t="s">
+        <v>212</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="57" t="s">
+        <v>217</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>214</v>
-      </c>
-      <c r="F4" s="60" t="s">
-        <v>215</v>
-      </c>
-      <c r="G4" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
+      <c r="C4" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="57" t="s">
-        <v>216</v>
+      <c r="B5" s="56" t="s">
+        <v>222</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -9174,9 +9234,9 @@
       <c r="I5" s="23"/>
     </row>
     <row r="6" ht="276" customHeight="1">
-      <c r="A6" s="62"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
       <c r="D6" s="23"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
@@ -9185,8 +9245,8 @@
       <c r="I6" s="23"/>
     </row>
     <row r="7" ht="315" customHeight="1">
-      <c r="A7" s="65"/>
-      <c r="B7" s="63"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="62"/>
       <c r="C7" s="37"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -9196,8 +9256,8 @@
       <c r="I7" s="23"/>
     </row>
     <row r="8" ht="333.75" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="63"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="62"/>
       <c r="C8" s="37"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -9208,7 +9268,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="57"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -9219,7 +9279,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="57"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -9230,7 +9290,7 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="57"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -9241,7 +9301,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="57"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -9252,7 +9312,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="57"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -9263,7 +9323,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="57"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -9274,7 +9334,7 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -9285,7 +9345,7 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="57"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -9296,7 +9356,7 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="57"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -9307,7 +9367,7 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="57"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -9318,7 +9378,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="57"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -9329,7 +9389,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -9340,7 +9400,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="23"/>
-      <c r="B21" s="57"/>
+      <c r="B21" s="56"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -9351,7 +9411,7 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="23"/>
-      <c r="B22" s="57"/>
+      <c r="B22" s="56"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -9362,7 +9422,7 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="23"/>
-      <c r="B23" s="57"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -9373,7 +9433,7 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="23"/>
-      <c r="B24" s="57"/>
+      <c r="B24" s="56"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -10385,17 +10445,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="56" t="str">
+      <c r="B1" s="55" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="66"/>
+      <c r="D1" s="65"/>
       <c r="E1" s="23"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -10413,142 +10473,142 @@
       <c r="E3" s="23"/>
     </row>
     <row r="4" ht="58.5" customHeight="1">
-      <c r="A4" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>221</v>
+      <c r="A4" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>226</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>214</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>227</v>
       </c>
       <c r="E4" s="23"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>222</v>
-      </c>
-      <c r="E5" s="61"/>
+      <c r="C5" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="60"/>
     </row>
     <row r="6" ht="160.5" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B6" s="57" t="s">
         <v>223</v>
       </c>
+      <c r="B6" s="56" t="s">
+        <v>229</v>
+      </c>
       <c r="C6" s="37" t="s">
-        <v>224</v>
+        <v>230</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="23"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="23"/>
-      <c r="B7" s="57"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="23"/>
       <c r="D7" s="37"/>
       <c r="E7" s="23"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="57"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="23"/>
       <c r="D8" s="37"/>
       <c r="E8" s="23"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="57"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="23"/>
       <c r="D9" s="37"/>
       <c r="E9" s="23"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="57"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="23"/>
       <c r="D10" s="37"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="57"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="23"/>
       <c r="D11" s="37"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="57"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="23"/>
       <c r="D12" s="37"/>
       <c r="E12" s="23"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="57"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="23"/>
       <c r="D13" s="37"/>
       <c r="E13" s="23"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="57"/>
+      <c r="B14" s="56"/>
       <c r="C14" s="23"/>
       <c r="D14" s="37"/>
       <c r="E14" s="23"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="57"/>
+      <c r="B15" s="56"/>
       <c r="C15" s="23"/>
       <c r="D15" s="37"/>
       <c r="E15" s="23"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="57"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="23"/>
       <c r="D16" s="37"/>
       <c r="E16" s="23"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="57"/>
+      <c r="B17" s="56"/>
       <c r="C17" s="23"/>
       <c r="D17" s="37"/>
       <c r="E17" s="23"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="57"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="23"/>
       <c r="D18" s="37"/>
       <c r="E18" s="23"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="57"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="23"/>
       <c r="D19" s="37"/>
       <c r="E19" s="23"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="23"/>
       <c r="D20" s="37"/>
       <c r="E20" s="23"/>
@@ -12742,25 +12802,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="67" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="67" t="s">
-        <v>227</v>
+      <c r="A1" s="66" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3">
@@ -12768,376 +12828,376 @@
         <v>185</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="36" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36"/>
       <c r="B14" s="36" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36"/>
       <c r="B15" s="36" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="36"/>
       <c r="B16" s="36" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36"/>
       <c r="B17" s="36" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36"/>
       <c r="B18" s="36" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="36"/>
       <c r="B19" s="36" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36"/>
       <c r="B20" s="36" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="36"/>
       <c r="B21" s="36" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="36"/>
       <c r="B22" s="36" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="36"/>
       <c r="B23" s="36" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="36"/>
       <c r="B24" s="36" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="36"/>
       <c r="B25" s="36" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="36"/>
       <c r="B26" s="36" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="36"/>
       <c r="B27" s="36" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="C27" s="36"/>
     </row>
     <row r="28">
       <c r="A28" s="36"/>
       <c r="B28" s="36" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C28" s="36"/>
     </row>
     <row r="29">
       <c r="A29" s="36"/>
       <c r="B29" s="36" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="C29" s="36"/>
     </row>
     <row r="30">
       <c r="A30" s="36"/>
       <c r="B30" s="36" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C30" s="36"/>
     </row>
     <row r="31">
       <c r="A31" s="36"/>
       <c r="B31" s="36" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="C31" s="36"/>
     </row>
     <row r="32">
       <c r="A32" s="36"/>
       <c r="B32" s="36" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C32" s="36"/>
     </row>
     <row r="33">
       <c r="A33" s="36"/>
       <c r="B33" s="36" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C33" s="36"/>
     </row>
     <row r="34">
       <c r="A34" s="36"/>
       <c r="B34" s="36" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="C34" s="36"/>
     </row>
     <row r="35">
       <c r="A35" s="36"/>
       <c r="B35" s="36" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C35" s="36"/>
     </row>
     <row r="36">
       <c r="A36" s="36"/>
       <c r="B36" s="36" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="C36" s="36"/>
     </row>
     <row r="37">
       <c r="A37" s="36"/>
       <c r="B37" s="36" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="C37" s="36"/>
     </row>
     <row r="38">
       <c r="A38" s="36"/>
       <c r="B38" s="36" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C38" s="36"/>
     </row>
     <row r="39">
       <c r="A39" s="36"/>
       <c r="B39" s="36" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="C39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="36"/>
       <c r="B40" s="36" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="36"/>
       <c r="B41" s="36" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="36"/>
       <c r="B42" s="36" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="C42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="36"/>
       <c r="B43" s="36" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="36"/>
       <c r="B44" s="36" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="C44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="36"/>
       <c r="B45" s="36" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="C45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="36"/>
       <c r="B46" s="36" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C46" s="36"/>
     </row>

</xml_diff>

<commit_message>
test configs for hierarchy
</commit_message>
<xml_diff>
--- a/dev-page/configs/sparnatural-hierarchy-config.xlsx
+++ b/dev-page/configs/sparnatural-hierarchy-config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
   <si>
     <r>
       <rPr>
@@ -695,6 +695,9 @@
   </si>
   <si>
     <t xml:space="preserve">exerce dans le quartier ou la voie</t>
+  </si>
+  <si>
+    <t>this:Personne_Organization_agentIsTargetOfPerformanceRelation_beginningDate</t>
   </si>
   <si>
     <t xml:space="preserve">(rico:agentIsTargetOfPerformanceRelation rico:beginningDate)</t>
@@ -6441,7 +6444,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
@@ -6742,7 +6745,7 @@
       <c r="AB8" s="47"/>
       <c r="AC8" s="47"/>
     </row>
-    <row r="9" ht="25.5">
+    <row r="9" ht="14.25">
       <c r="A9" s="49" t="str">
         <f>CONCATENATE("this:",RIGHT(C9,LEN(C9)-SEARCH(":",C9)),"_",RIGHT(B9,LEN(B9)-SEARCH(":",B9)))</f>
         <v>this:Place_hasOrHadPlaceType</v>
@@ -7265,7 +7268,7 @@
       <c r="AB24" s="47"/>
       <c r="AC24" s="47"/>
     </row>
-    <row r="25" ht="15">
+    <row r="25" ht="14.25">
       <c r="A25" s="49" t="str">
         <f>CONCATENATE("this:",RIGHT(C25,LEN(C25)-SEARCH(":",C25)),"_",RIGHT(B25,LEN(B25)-SEARCH(":",B25)))</f>
         <v>this:Adresse_hasOrHadLocation</v>
@@ -7473,7 +7476,7 @@
       <c r="H30" s="17"/>
       <c r="O30" s="7"/>
     </row>
-    <row r="31" ht="15">
+    <row r="31" ht="15.75">
       <c r="A31" s="46" t="s">
         <v>121</v>
       </c>
@@ -7506,33 +7509,32 @@
       <c r="AB31" s="47"/>
       <c r="AC31" s="47"/>
     </row>
-    <row r="32" ht="15">
-      <c r="A32" s="49" t="str">
-        <f>CONCATENATE("this:",RIGHT(C32,LEN(C32)-SEARCH(":",C32)),"_",RIGHT(B32,LEN(B32)-SEARCH(":",B32)))</f>
-        <v xml:space="preserve">this:Personne, this:Organization_agentIsTargetOfPerformanceRelation rico:beginningDate)</v>
+    <row r="32" ht="28.5">
+      <c r="A32" s="53" t="s">
+        <v>206</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F32" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="K32" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L32" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O32" s="7" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="33" ht="15">
@@ -9168,22 +9170,22 @@
     </row>
     <row r="3" ht="91.5" customHeight="1">
       <c r="A3" s="57" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B3" s="57" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D3" s="57" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E3" s="57" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F3" s="57" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -9197,19 +9199,19 @@
         <v>27</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D4" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="G4" s="59" t="s">
         <v>219</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>218</v>
       </c>
       <c r="H4" s="60"/>
       <c r="I4" s="60"/>
@@ -9219,14 +9221,14 @@
         <v>194</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -10474,16 +10476,16 @@
     </row>
     <row r="4" ht="58.5" customHeight="1">
       <c r="A4" s="57" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B4" s="57" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D4" s="57" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E4" s="23"/>
     </row>
@@ -10495,22 +10497,22 @@
         <v>27</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E5" s="60"/>
     </row>
     <row r="6" ht="160.5" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B6" s="56" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="23"/>
@@ -12803,24 +12805,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="66" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C1" s="66" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3">
@@ -12828,376 +12830,376 @@
         <v>185</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36"/>
       <c r="B14" s="36" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36"/>
       <c r="B15" s="36" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="36"/>
       <c r="B16" s="36" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36"/>
       <c r="B17" s="36" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36"/>
       <c r="B18" s="36" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="36"/>
       <c r="B19" s="36" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36"/>
       <c r="B20" s="36" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="36"/>
       <c r="B21" s="36" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="36"/>
       <c r="B22" s="36" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="36"/>
       <c r="B23" s="36" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="36"/>
       <c r="B24" s="36" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="36"/>
       <c r="B25" s="36" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="36"/>
       <c r="B26" s="36" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="36"/>
       <c r="B27" s="36" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C27" s="36"/>
     </row>
     <row r="28">
       <c r="A28" s="36"/>
       <c r="B28" s="36" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C28" s="36"/>
     </row>
     <row r="29">
       <c r="A29" s="36"/>
       <c r="B29" s="36" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C29" s="36"/>
     </row>
     <row r="30">
       <c r="A30" s="36"/>
       <c r="B30" s="36" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C30" s="36"/>
     </row>
     <row r="31">
       <c r="A31" s="36"/>
       <c r="B31" s="36" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C31" s="36"/>
     </row>
     <row r="32">
       <c r="A32" s="36"/>
       <c r="B32" s="36" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C32" s="36"/>
     </row>
     <row r="33">
       <c r="A33" s="36"/>
       <c r="B33" s="36" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C33" s="36"/>
     </row>
     <row r="34">
       <c r="A34" s="36"/>
       <c r="B34" s="36" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C34" s="36"/>
     </row>
     <row r="35">
       <c r="A35" s="36"/>
       <c r="B35" s="36" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C35" s="36"/>
     </row>
     <row r="36">
       <c r="A36" s="36"/>
       <c r="B36" s="36" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C36" s="36"/>
     </row>
     <row r="37">
       <c r="A37" s="36"/>
       <c r="B37" s="36" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C37" s="36"/>
     </row>
     <row r="38">
       <c r="A38" s="36"/>
       <c r="B38" s="36" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C38" s="36"/>
     </row>
     <row r="39">
       <c r="A39" s="36"/>
       <c r="B39" s="36" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="36"/>
       <c r="B40" s="36" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="36"/>
       <c r="B41" s="36" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="36"/>
       <c r="B42" s="36" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="36"/>
       <c r="B43" s="36" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="36"/>
       <c r="B44" s="36" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="36"/>
       <c r="B45" s="36" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="36"/>
       <c r="B46" s="36" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C46" s="36"/>
     </row>

</xml_diff>

<commit_message>
Fix property reading + added test for property hierarchy
</commit_message>
<xml_diff>
--- a/dev-page/configs/sparnatural-hierarchy-config.xlsx
+++ b/dev-page/configs/sparnatural-hierarchy-config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="323">
   <si>
     <r>
       <rPr>
@@ -716,6 +716,30 @@
   </si>
   <si>
     <t>core:TimeProperty-Date</t>
+  </si>
+  <si>
+    <t>this:Personne_beginningDate</t>
+  </si>
+  <si>
+    <t>rico:beginningDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has beginning date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a pour date de début</t>
+  </si>
+  <si>
+    <t>this:Personne_birthDate</t>
+  </si>
+  <si>
+    <t>rico:birthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">has birth date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date de naissance</t>
   </si>
   <si>
     <t xml:space="preserve">URI of the datasource in the configuration. This is the value that should be referenced from the "datasources:datasource" column in the properties tab</t>
@@ -1331,7 +1355,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1447,6 +1471,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf fontId="26" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="20" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -7537,17 +7564,71 @@
         <v>212</v>
       </c>
     </row>
-    <row r="33" ht="15">
-      <c r="C33" s="17"/>
+    <row r="33" ht="14.25">
+      <c r="A33" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="B33" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="34"/>
+      <c r="E33" s="54" t="s">
+        <v>215</v>
+      </c>
+      <c r="F33" s="54" t="s">
+        <v>216</v>
+      </c>
       <c r="G33" s="17"/>
       <c r="H33" s="17"/>
-      <c r="O33" s="7"/>
-    </row>
-    <row r="34" ht="15">
-      <c r="C34" s="17"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="L33" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
+      <c r="O33" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="A34" s="53" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="34"/>
+      <c r="E34" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="F34" s="54" t="s">
+        <v>220</v>
+      </c>
       <c r="G34" s="17"/>
       <c r="H34" s="17"/>
-      <c r="O34" s="7"/>
+      <c r="I34" s="34"/>
+      <c r="J34" s="34"/>
+      <c r="K34" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="L34" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="M34" s="34"/>
+      <c r="N34" s="34"/>
+      <c r="O34" s="7" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="35" ht="15">
       <c r="C35" s="17"/>
@@ -9062,8 +9143,8 @@
     <row r="946" ht="15"/>
     <row r="947" ht="15"/>
   </sheetData>
-  <dataValidations count="14" disablePrompts="0">
-    <dataValidation sqref="O27 O30 O32:O45" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+  <dataValidations count="16" disablePrompts="0">
+    <dataValidation sqref="O27 O30 O32 O35:O45" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
       <formula1>'sparnatural-config-core'!$A$2:$A$13</formula1>
     </dataValidation>
     <dataValidation sqref="O9" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
@@ -9105,6 +9186,12 @@
     <dataValidation sqref="O29" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="0" showInputMessage="0">
       <formula1>'sparnatural-config-core'!$A$2:$A$12</formula1>
     </dataValidation>
+    <dataValidation sqref="O33" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>'sparnatural-config-core'!$A$2:$A$13</formula1>
+    </dataValidation>
+    <dataValidation sqref="O34" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+      <formula1>'sparnatural-config-core'!$A$2:$A$13</formula1>
+    </dataValidation>
   </dataValidations>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.78750000000000009" right="0.78750000000000009" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -9140,18 +9227,18 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="55" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>138</v>
       </c>
       <c r="D1" s="23"/>
-      <c r="E1" s="56"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
@@ -9169,66 +9256,66 @@
       <c r="I2" s="23"/>
     </row>
     <row r="3" ht="91.5" customHeight="1">
-      <c r="A3" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>214</v>
-      </c>
-      <c r="C3" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="57" t="s">
-        <v>216</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>217</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>218</v>
+      <c r="A3" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>226</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="C4" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>228</v>
+      </c>
+      <c r="E4" s="60" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="60" t="s">
+        <v>230</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>227</v>
+      </c>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="34" t="s">
         <v>194</v>
       </c>
-      <c r="B5" s="56" t="s">
-        <v>223</v>
+      <c r="B5" s="57" t="s">
+        <v>231</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
@@ -9236,9 +9323,9 @@
       <c r="I5" s="23"/>
     </row>
     <row r="6" ht="276" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
+      <c r="A6" s="62"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="23"/>
       <c r="E6" s="34"/>
       <c r="F6" s="34"/>
@@ -9247,8 +9334,8 @@
       <c r="I6" s="23"/>
     </row>
     <row r="7" ht="315" customHeight="1">
-      <c r="A7" s="64"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="63"/>
       <c r="C7" s="37"/>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -9258,8 +9345,8 @@
       <c r="I7" s="23"/>
     </row>
     <row r="8" ht="333.75" customHeight="1">
-      <c r="A8" s="64"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="37"/>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
@@ -9270,7 +9357,7 @@
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -9281,7 +9368,7 @@
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
@@ -9292,7 +9379,7 @@
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -9303,7 +9390,7 @@
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="23"/>
@@ -9314,7 +9401,7 @@
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -9325,7 +9412,7 @@
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
@@ -9336,7 +9423,7 @@
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -9347,7 +9434,7 @@
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -9358,7 +9445,7 @@
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -9369,7 +9456,7 @@
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -9380,7 +9467,7 @@
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="23"/>
@@ -9391,7 +9478,7 @@
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
@@ -9402,7 +9489,7 @@
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="23"/>
-      <c r="B21" s="56"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -9413,7 +9500,7 @@
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="23"/>
-      <c r="B22" s="56"/>
+      <c r="B22" s="57"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
       <c r="E22" s="23"/>
@@ -9424,7 +9511,7 @@
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="23"/>
-      <c r="B23" s="56"/>
+      <c r="B23" s="57"/>
       <c r="C23" s="23"/>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -9435,7 +9522,7 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="23"/>
-      <c r="B24" s="56"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
       <c r="E24" s="23"/>
@@ -10447,17 +10534,17 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="55" t="str">
+      <c r="B1" s="56" t="str">
         <f>Entities!B1</f>
         <v>http://data.mydomain.com/sparnatural-page/sparnatural-config</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="D1" s="65"/>
+      <c r="D1" s="66"/>
       <c r="E1" s="23"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
@@ -10475,142 +10562,142 @@
       <c r="E3" s="23"/>
     </row>
     <row r="4" ht="58.5" customHeight="1">
-      <c r="A4" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="B4" s="57" t="s">
+      <c r="A4" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="E4" s="23"/>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="C4" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="E4" s="23"/>
-    </row>
-    <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" s="60"/>
+      <c r="D5" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="61"/>
     </row>
     <row r="6" ht="160.5" customHeight="1">
       <c r="A6" s="23" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>230</v>
+        <v>232</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>238</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="23"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="23"/>
-      <c r="B7" s="56"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="23"/>
       <c r="D7" s="37"/>
       <c r="E7" s="23"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="23"/>
       <c r="D8" s="37"/>
       <c r="E8" s="23"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="23"/>
-      <c r="B9" s="56"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="23"/>
       <c r="D9" s="37"/>
       <c r="E9" s="23"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="56"/>
+      <c r="B10" s="57"/>
       <c r="C10" s="23"/>
       <c r="D10" s="37"/>
       <c r="E10" s="23"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="23"/>
-      <c r="B11" s="56"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="23"/>
       <c r="D11" s="37"/>
       <c r="E11" s="23"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="23"/>
-      <c r="B12" s="56"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="23"/>
       <c r="D12" s="37"/>
       <c r="E12" s="23"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="23"/>
-      <c r="B13" s="56"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="23"/>
       <c r="D13" s="37"/>
       <c r="E13" s="23"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="23"/>
-      <c r="B14" s="56"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="23"/>
       <c r="D14" s="37"/>
       <c r="E14" s="23"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="23"/>
-      <c r="B15" s="56"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="23"/>
       <c r="D15" s="37"/>
       <c r="E15" s="23"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="23"/>
-      <c r="B16" s="56"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="23"/>
       <c r="D16" s="37"/>
       <c r="E16" s="23"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="23"/>
-      <c r="B17" s="56"/>
+      <c r="B17" s="57"/>
       <c r="C17" s="23"/>
       <c r="D17" s="37"/>
       <c r="E17" s="23"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="23"/>
-      <c r="B18" s="56"/>
+      <c r="B18" s="57"/>
       <c r="C18" s="23"/>
       <c r="D18" s="37"/>
       <c r="E18" s="23"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="23"/>
-      <c r="B19" s="56"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="23"/>
       <c r="D19" s="37"/>
       <c r="E19" s="23"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="23"/>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="23"/>
       <c r="D20" s="37"/>
       <c r="E20" s="23"/>
@@ -12804,25 +12891,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="66" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="66" t="s">
-        <v>233</v>
-      </c>
-      <c r="C1" s="66" t="s">
-        <v>234</v>
+      <c r="A1" s="67" t="s">
+        <v>240</v>
+      </c>
+      <c r="B1" s="67" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1" s="67" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3">
@@ -12830,10 +12917,10 @@
         <v>185</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="4">
@@ -12841,365 +12928,365 @@
         <v>212</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="36" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="36" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="36" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="36" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="36" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="36" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="36" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>264</v>
+        <v>272</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>268</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36"/>
       <c r="B14" s="36" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C14" s="36" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36"/>
       <c r="B15" s="36" t="s">
-        <v>271</v>
+        <v>279</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="36"/>
       <c r="B16" s="36" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="36"/>
       <c r="B17" s="36" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C17" s="36" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="36"/>
       <c r="B18" s="36" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C18" s="36" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="36"/>
       <c r="B19" s="36" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C19" s="36" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36"/>
       <c r="B20" s="36" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C20" s="36" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="36"/>
       <c r="B21" s="36" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="36"/>
       <c r="B22" s="36" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C22" s="36" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="36"/>
       <c r="B23" s="36" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="36"/>
       <c r="B24" s="36" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="36"/>
       <c r="B25" s="36" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="36"/>
       <c r="B26" s="36" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C26" s="36" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="36"/>
       <c r="B27" s="36" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C27" s="36"/>
     </row>
     <row r="28">
       <c r="A28" s="36"/>
       <c r="B28" s="36" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C28" s="36"/>
     </row>
     <row r="29">
       <c r="A29" s="36"/>
       <c r="B29" s="36" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C29" s="36"/>
     </row>
     <row r="30">
       <c r="A30" s="36"/>
       <c r="B30" s="36" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C30" s="36"/>
     </row>
     <row r="31">
       <c r="A31" s="36"/>
       <c r="B31" s="36" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C31" s="36"/>
     </row>
     <row r="32">
       <c r="A32" s="36"/>
       <c r="B32" s="36" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C32" s="36"/>
     </row>
     <row r="33">
       <c r="A33" s="36"/>
       <c r="B33" s="36" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="C33" s="36"/>
     </row>
     <row r="34">
       <c r="A34" s="36"/>
       <c r="B34" s="36" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C34" s="36"/>
     </row>
     <row r="35">
       <c r="A35" s="36"/>
       <c r="B35" s="36" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C35" s="36"/>
     </row>
     <row r="36">
       <c r="A36" s="36"/>
       <c r="B36" s="36" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C36" s="36"/>
     </row>
     <row r="37">
       <c r="A37" s="36"/>
       <c r="B37" s="36" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C37" s="36"/>
     </row>
     <row r="38">
       <c r="A38" s="36"/>
       <c r="B38" s="36" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C38" s="36"/>
     </row>
     <row r="39">
       <c r="A39" s="36"/>
       <c r="B39" s="36" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C39" s="36"/>
     </row>
     <row r="40">
       <c r="A40" s="36"/>
       <c r="B40" s="36" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C40" s="36"/>
     </row>
     <row r="41">
       <c r="A41" s="36"/>
       <c r="B41" s="36" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C41" s="36"/>
     </row>
     <row r="42">
       <c r="A42" s="36"/>
       <c r="B42" s="36" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C42" s="36"/>
     </row>
     <row r="43">
       <c r="A43" s="36"/>
       <c r="B43" s="36" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="C43" s="36"/>
     </row>
     <row r="44">
       <c r="A44" s="36"/>
       <c r="B44" s="36" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="C44" s="36"/>
     </row>
     <row r="45">
       <c r="A45" s="36"/>
       <c r="B45" s="36" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
       <c r="C45" s="36"/>
     </row>
     <row r="46">
       <c r="A46" s="36"/>
       <c r="B46" s="36" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C46" s="36"/>
     </row>

</xml_diff>